<commit_message>
change mqome parameters to 2 min_peptides, min_pep_nsmap 'all', min_child_nsamp 0
</commit_message>
<xml_diff>
--- a/results/legacy/rank_tables_comparison.xlsx
+++ b/results/legacy/rank_tables_comparison.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rsajulga/Projects/umn/galaxyp/functional-tools-survey/functional-analysis-benchmarking/results/legacy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13AB10F5-4F66-BE4D-A725-AFA970588995}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{408F095F-8CD5-984A-8578-A4AE7E07C9E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="580" yWindow="640" windowWidth="32140" windowHeight="16640" xr2:uid="{0B4038EE-9BFE-1546-B252-9856E1BA96F5}"/>
+    <workbookView xWindow="-560" yWindow="460" windowWidth="32780" windowHeight="18320" activeTab="1" xr2:uid="{0B4038EE-9BFE-1546-B252-9856E1BA96F5}"/>
   </bookViews>
   <sheets>
     <sheet name="040720" sheetId="1" r:id="rId1"/>
+    <sheet name="041420" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1148" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2288" uniqueCount="394">
   <si>
     <t>GO Term</t>
   </si>
@@ -1056,6 +1057,165 @@
   </si>
   <si>
     <t>0.39 (9.84 / 7.26)</t>
+  </si>
+  <si>
+    <t>0.06 (-10.76 / -10.37)</t>
+  </si>
+  <si>
+    <t>Ras GTPase binding</t>
+  </si>
+  <si>
+    <t>0.88 (3.58 / 1.49)</t>
+  </si>
+  <si>
+    <t>0.03 (3.58 / 3.49)</t>
+  </si>
+  <si>
+    <t>0.83 (6.54 / 3.23)</t>
+  </si>
+  <si>
+    <t>0.22 (7.5 / 6.28)</t>
+  </si>
+  <si>
+    <t>0.24 (7.04 / 5.81)</t>
+  </si>
+  <si>
+    <t>0.11 (4.91 / 4.49)</t>
+  </si>
+  <si>
+    <t>small GTPase binding</t>
+  </si>
+  <si>
+    <t>0.81 (4.09 / 1.91)</t>
+  </si>
+  <si>
+    <t>endoribonuclease activity, producing 5'-phosphomonoesters</t>
+  </si>
+  <si>
+    <t>0.73 (3.81 / 1.91)</t>
+  </si>
+  <si>
+    <t>0.13 (4.17 / 3.71)</t>
+  </si>
+  <si>
+    <t>0.33 (6.55 / 5)</t>
+  </si>
+  <si>
+    <t>0.09 (5.64 / 5.23)</t>
+  </si>
+  <si>
+    <t>exodeoxyribonuclease activity, producing 5'-phosphomonoesters</t>
+  </si>
+  <si>
+    <t>0.68 (5.25 / 2.91)</t>
+  </si>
+  <si>
+    <t>0.12 (6.04 / 5.49)</t>
+  </si>
+  <si>
+    <t>-0.2 (5.86 / 6.88)</t>
+  </si>
+  <si>
+    <t>0.08 (5.32 / 4.99)</t>
+  </si>
+  <si>
+    <t>GTPase binding</t>
+  </si>
+  <si>
+    <t>hexokinase activity</t>
+  </si>
+  <si>
+    <t>0.39 (6.7 / 4.86)</t>
+  </si>
+  <si>
+    <t>0.35 (7.6 / 5.75)</t>
+  </si>
+  <si>
+    <t>sequence-specific double-stranded DNA binding</t>
+  </si>
+  <si>
+    <t>0.33 (5.39 / 4.08)</t>
+  </si>
+  <si>
+    <t>-0.46 (4.39 / 6.4)</t>
+  </si>
+  <si>
+    <t>0.27 (5 / 3.99)</t>
+  </si>
+  <si>
+    <t>0.29 (7.56 / 6)</t>
+  </si>
+  <si>
+    <t>-0.43 (-8.73 / -11.43)</t>
+  </si>
+  <si>
+    <t>monocarboxylic acid binding</t>
+  </si>
+  <si>
+    <t>0.3 (8.12 / 6.43)</t>
+  </si>
+  <si>
+    <t>-0.01 (7.04 / 7.09)</t>
+  </si>
+  <si>
+    <t>0.19 (7.61 / 6.58)</t>
+  </si>
+  <si>
+    <t>0.25 (8.9 / 7.3)</t>
+  </si>
+  <si>
+    <t>deaminase activity</t>
+  </si>
+  <si>
+    <t>0.28 (5.67 / 4.49)</t>
+  </si>
+  <si>
+    <t>-0.35 (4.39 / 5.86)</t>
+  </si>
+  <si>
+    <t>0.01 (8.2 / 8.11)</t>
+  </si>
+  <si>
+    <t>0.11 (6.97 / 6.38)</t>
+  </si>
+  <si>
+    <t>0.24 (9.92 / 8.25)</t>
+  </si>
+  <si>
+    <t>0.13 (-6.5 / -6.03)</t>
+  </si>
+  <si>
+    <t>endodeoxyribonuclease activity, producing 5'-phosphomonoesters</t>
+  </si>
+  <si>
+    <t>0.27 (5.91 / 4.71)</t>
+  </si>
+  <si>
+    <t>-0.48 (4.64 / 6.87)</t>
+  </si>
+  <si>
+    <t>-0.23 (5.86 / 7.04)</t>
+  </si>
+  <si>
+    <t>oxidoreductase activity, acting on other nitrogenous compounds as donors, with NAD or NADP as acceptor</t>
+  </si>
+  <si>
+    <t>0.25 (6.09 / 4.95)</t>
+  </si>
+  <si>
+    <t>C-methyltransferase activity</t>
+  </si>
+  <si>
+    <t>0.25 (5.64 / 4.61)</t>
+  </si>
+  <si>
+    <t>0.24 (6.29 / 5.15)</t>
+  </si>
+  <si>
+    <t>0.23 (6.55 / 5.43)</t>
+  </si>
+  <si>
+    <t>0.19 (6.64 / 5.7)</t>
   </si>
 </sst>
 </file>
@@ -1427,8 +1587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0972C2C-480C-B444-8AFD-83D83643B809}">
   <dimension ref="B1:R104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B50" workbookViewId="0">
-      <selection activeCell="K76" sqref="K76"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5908,4 +6068,4491 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B929CB3-0F32-FC4E-9739-69EA2331ACF1}">
+  <dimension ref="B1:R104"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="24.33203125" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" customWidth="1"/>
+    <col min="11" max="11" width="25.6640625" customWidth="1"/>
+    <col min="12" max="12" width="18.83203125" customWidth="1"/>
+    <col min="13" max="13" width="20.5" customWidth="1"/>
+    <col min="14" max="14" width="18.33203125" customWidth="1"/>
+    <col min="15" max="15" width="25.1640625" customWidth="1"/>
+    <col min="16" max="16" width="12.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B1" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="3" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B3" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" t="s">
+        <v>2</v>
+      </c>
+      <c r="K4" t="s">
+        <v>0</v>
+      </c>
+      <c r="L4" t="s">
+        <v>1</v>
+      </c>
+      <c r="M4" t="s">
+        <v>3</v>
+      </c>
+      <c r="N4" t="s">
+        <v>4</v>
+      </c>
+      <c r="O4" t="s">
+        <v>5</v>
+      </c>
+      <c r="P4" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>7</v>
+      </c>
+      <c r="R4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" t="s">
+        <v>86</v>
+      </c>
+      <c r="H5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K5" t="s">
+        <v>131</v>
+      </c>
+      <c r="L5" t="s">
+        <v>24</v>
+      </c>
+      <c r="M5" t="s">
+        <v>132</v>
+      </c>
+      <c r="N5" t="s">
+        <v>133</v>
+      </c>
+      <c r="O5" t="s">
+        <v>9</v>
+      </c>
+      <c r="P5" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>9</v>
+      </c>
+      <c r="R5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="E6">
+        <v>13.887</v>
+      </c>
+      <c r="F6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6">
+        <v>71.875</v>
+      </c>
+      <c r="H6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" t="s">
+        <v>9</v>
+      </c>
+      <c r="L6" t="s">
+        <v>29</v>
+      </c>
+      <c r="M6">
+        <v>0.313</v>
+      </c>
+      <c r="N6">
+        <v>39.011000000000003</v>
+      </c>
+      <c r="O6" t="s">
+        <v>9</v>
+      </c>
+      <c r="P6" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>9</v>
+      </c>
+      <c r="R6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>88</v>
+      </c>
+      <c r="E7" t="s">
+        <v>89</v>
+      </c>
+      <c r="F7" t="s">
+        <v>90</v>
+      </c>
+      <c r="G7" t="s">
+        <v>91</v>
+      </c>
+      <c r="H7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7" t="s">
+        <v>92</v>
+      </c>
+      <c r="K7" t="s">
+        <v>143</v>
+      </c>
+      <c r="L7" t="s">
+        <v>24</v>
+      </c>
+      <c r="M7" t="s">
+        <v>144</v>
+      </c>
+      <c r="N7" t="s">
+        <v>145</v>
+      </c>
+      <c r="O7" t="s">
+        <v>146</v>
+      </c>
+      <c r="P7" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>341</v>
+      </c>
+      <c r="R7" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="E8">
+        <v>33.043999999999997</v>
+      </c>
+      <c r="F8">
+        <v>37.85</v>
+      </c>
+      <c r="G8">
+        <v>43.466000000000001</v>
+      </c>
+      <c r="H8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I8">
+        <v>33.994999999999997</v>
+      </c>
+      <c r="L8" t="s">
+        <v>29</v>
+      </c>
+      <c r="M8">
+        <v>0.627</v>
+      </c>
+      <c r="N8">
+        <v>34.341000000000001</v>
+      </c>
+      <c r="O8">
+        <v>74.271000000000001</v>
+      </c>
+      <c r="P8" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q8">
+        <v>16.111000000000001</v>
+      </c>
+      <c r="R8">
+        <v>97.507999999999996</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" t="s">
+        <v>94</v>
+      </c>
+      <c r="E9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9" t="s">
+        <v>9</v>
+      </c>
+      <c r="K9" t="s">
+        <v>148</v>
+      </c>
+      <c r="L9" t="s">
+        <v>24</v>
+      </c>
+      <c r="M9" t="s">
+        <v>149</v>
+      </c>
+      <c r="N9" t="s">
+        <v>150</v>
+      </c>
+      <c r="O9" t="s">
+        <v>151</v>
+      </c>
+      <c r="P9" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>9</v>
+      </c>
+      <c r="R9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10">
+        <v>0.21299999999999999</v>
+      </c>
+      <c r="E10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" t="s">
+        <v>9</v>
+      </c>
+      <c r="I10" t="s">
+        <v>9</v>
+      </c>
+      <c r="L10" t="s">
+        <v>29</v>
+      </c>
+      <c r="M10">
+        <v>0.94</v>
+      </c>
+      <c r="N10">
+        <v>15.385</v>
+      </c>
+      <c r="O10">
+        <v>10.875</v>
+      </c>
+      <c r="P10" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>9</v>
+      </c>
+      <c r="R10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>95</v>
+      </c>
+      <c r="C11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" t="s">
+        <v>94</v>
+      </c>
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" t="s">
+        <v>9</v>
+      </c>
+      <c r="I11" t="s">
+        <v>9</v>
+      </c>
+      <c r="K11" t="s">
+        <v>342</v>
+      </c>
+      <c r="L11" t="s">
+        <v>24</v>
+      </c>
+      <c r="M11" t="s">
+        <v>343</v>
+      </c>
+      <c r="N11" t="s">
+        <v>9</v>
+      </c>
+      <c r="O11" t="s">
+        <v>9</v>
+      </c>
+      <c r="P11" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>9</v>
+      </c>
+      <c r="R11" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12">
+        <v>0.28299999999999997</v>
+      </c>
+      <c r="E12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" t="s">
+        <v>9</v>
+      </c>
+      <c r="H12" t="s">
+        <v>9</v>
+      </c>
+      <c r="I12" t="s">
+        <v>9</v>
+      </c>
+      <c r="L12" t="s">
+        <v>29</v>
+      </c>
+      <c r="M12">
+        <v>1.254</v>
+      </c>
+      <c r="N12" t="s">
+        <v>9</v>
+      </c>
+      <c r="O12" t="s">
+        <v>9</v>
+      </c>
+      <c r="P12" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>9</v>
+      </c>
+      <c r="R12">
+        <v>42.055999999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>96</v>
+      </c>
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" t="s">
+        <v>94</v>
+      </c>
+      <c r="E13" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" t="s">
+        <v>97</v>
+      </c>
+      <c r="G13" t="s">
+        <v>9</v>
+      </c>
+      <c r="H13" t="s">
+        <v>9</v>
+      </c>
+      <c r="I13" t="s">
+        <v>9</v>
+      </c>
+      <c r="K13" t="s">
+        <v>103</v>
+      </c>
+      <c r="L13" t="s">
+        <v>24</v>
+      </c>
+      <c r="M13" t="s">
+        <v>345</v>
+      </c>
+      <c r="N13" t="s">
+        <v>346</v>
+      </c>
+      <c r="O13" t="s">
+        <v>347</v>
+      </c>
+      <c r="P13" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>9</v>
+      </c>
+      <c r="R13" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14">
+        <v>0.35399999999999998</v>
+      </c>
+      <c r="E14">
+        <v>29.076000000000001</v>
+      </c>
+      <c r="F14">
+        <v>74.533000000000001</v>
+      </c>
+      <c r="G14" t="s">
+        <v>9</v>
+      </c>
+      <c r="H14" t="s">
+        <v>9</v>
+      </c>
+      <c r="I14" t="s">
+        <v>9</v>
+      </c>
+      <c r="L14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M14">
+        <v>1.5669999999999999</v>
+      </c>
+      <c r="N14">
+        <v>10.989000000000001</v>
+      </c>
+      <c r="O14">
+        <v>7.6920000000000002</v>
+      </c>
+      <c r="P14" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>9</v>
+      </c>
+      <c r="R14">
+        <v>19.315000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>98</v>
+      </c>
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" t="s">
+        <v>99</v>
+      </c>
+      <c r="E15" t="s">
+        <v>100</v>
+      </c>
+      <c r="F15" t="s">
+        <v>101</v>
+      </c>
+      <c r="G15" t="s">
+        <v>9</v>
+      </c>
+      <c r="H15" t="s">
+        <v>9</v>
+      </c>
+      <c r="I15" t="s">
+        <v>102</v>
+      </c>
+      <c r="K15" t="s">
+        <v>349</v>
+      </c>
+      <c r="L15" t="s">
+        <v>24</v>
+      </c>
+      <c r="M15" t="s">
+        <v>350</v>
+      </c>
+      <c r="N15" t="s">
+        <v>9</v>
+      </c>
+      <c r="O15" t="s">
+        <v>9</v>
+      </c>
+      <c r="P15" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>9</v>
+      </c>
+      <c r="R15" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16">
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="E16">
+        <v>5.0839999999999996</v>
+      </c>
+      <c r="F16">
+        <v>12.967000000000001</v>
+      </c>
+      <c r="G16" t="s">
+        <v>9</v>
+      </c>
+      <c r="H16" t="s">
+        <v>9</v>
+      </c>
+      <c r="I16">
+        <v>3.1560000000000001</v>
+      </c>
+      <c r="L16" t="s">
+        <v>29</v>
+      </c>
+      <c r="M16">
+        <v>1.881</v>
+      </c>
+      <c r="N16" t="s">
+        <v>9</v>
+      </c>
+      <c r="O16" t="s">
+        <v>9</v>
+      </c>
+      <c r="P16" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>9</v>
+      </c>
+      <c r="R16">
+        <v>42.368000000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>103</v>
+      </c>
+      <c r="C17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" t="s">
+        <v>104</v>
+      </c>
+      <c r="E17" t="s">
+        <v>105</v>
+      </c>
+      <c r="F17" t="s">
+        <v>106</v>
+      </c>
+      <c r="G17" t="s">
+        <v>9</v>
+      </c>
+      <c r="H17" t="s">
+        <v>9</v>
+      </c>
+      <c r="I17" t="s">
+        <v>107</v>
+      </c>
+      <c r="K17" t="s">
+        <v>185</v>
+      </c>
+      <c r="L17" t="s">
+        <v>24</v>
+      </c>
+      <c r="M17" t="s">
+        <v>187</v>
+      </c>
+      <c r="N17" t="s">
+        <v>9</v>
+      </c>
+      <c r="O17" t="s">
+        <v>188</v>
+      </c>
+      <c r="P17" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>9</v>
+      </c>
+      <c r="R17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18">
+        <v>0.496</v>
+      </c>
+      <c r="E18">
+        <v>30.687999999999999</v>
+      </c>
+      <c r="F18">
+        <v>36.215000000000003</v>
+      </c>
+      <c r="G18" t="s">
+        <v>9</v>
+      </c>
+      <c r="H18" t="s">
+        <v>9</v>
+      </c>
+      <c r="I18">
+        <v>79.981999999999999</v>
+      </c>
+      <c r="L18" t="s">
+        <v>29</v>
+      </c>
+      <c r="M18">
+        <v>2.194</v>
+      </c>
+      <c r="N18" t="s">
+        <v>9</v>
+      </c>
+      <c r="O18">
+        <v>2.653</v>
+      </c>
+      <c r="P18" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>9</v>
+      </c>
+      <c r="R18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>108</v>
+      </c>
+      <c r="C19" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" t="s">
+        <v>109</v>
+      </c>
+      <c r="E19" t="s">
+        <v>110</v>
+      </c>
+      <c r="F19" t="s">
+        <v>9</v>
+      </c>
+      <c r="G19" t="s">
+        <v>9</v>
+      </c>
+      <c r="H19" t="s">
+        <v>9</v>
+      </c>
+      <c r="I19" t="s">
+        <v>9</v>
+      </c>
+      <c r="K19" t="s">
+        <v>351</v>
+      </c>
+      <c r="L19" t="s">
+        <v>24</v>
+      </c>
+      <c r="M19" t="s">
+        <v>352</v>
+      </c>
+      <c r="N19" t="s">
+        <v>353</v>
+      </c>
+      <c r="O19" t="s">
+        <v>354</v>
+      </c>
+      <c r="P19" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>9</v>
+      </c>
+      <c r="R19" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="20" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20">
+        <v>0.56699999999999995</v>
+      </c>
+      <c r="E20">
+        <v>10.911</v>
+      </c>
+      <c r="F20" t="s">
+        <v>9</v>
+      </c>
+      <c r="G20" t="s">
+        <v>9</v>
+      </c>
+      <c r="H20" t="s">
+        <v>9</v>
+      </c>
+      <c r="I20" t="s">
+        <v>9</v>
+      </c>
+      <c r="L20" t="s">
+        <v>29</v>
+      </c>
+      <c r="M20">
+        <v>2.508</v>
+      </c>
+      <c r="N20">
+        <v>17.856999999999999</v>
+      </c>
+      <c r="O20">
+        <v>4.7750000000000004</v>
+      </c>
+      <c r="P20" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>9</v>
+      </c>
+      <c r="R20">
+        <v>20.561</v>
+      </c>
+    </row>
+    <row r="21" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>111</v>
+      </c>
+      <c r="C21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" t="s">
+        <v>112</v>
+      </c>
+      <c r="E21" t="s">
+        <v>113</v>
+      </c>
+      <c r="F21" t="s">
+        <v>114</v>
+      </c>
+      <c r="G21" t="s">
+        <v>9</v>
+      </c>
+      <c r="H21" t="s">
+        <v>9</v>
+      </c>
+      <c r="I21" t="s">
+        <v>115</v>
+      </c>
+      <c r="K21" t="s">
+        <v>356</v>
+      </c>
+      <c r="L21" t="s">
+        <v>24</v>
+      </c>
+      <c r="M21" t="s">
+        <v>357</v>
+      </c>
+      <c r="N21" t="s">
+        <v>358</v>
+      </c>
+      <c r="O21" t="s">
+        <v>359</v>
+      </c>
+      <c r="P21" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>9</v>
+      </c>
+      <c r="R21" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="22" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C22" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22">
+        <v>0.63800000000000001</v>
+      </c>
+      <c r="E22">
+        <v>41.970999999999997</v>
+      </c>
+      <c r="F22">
+        <v>74.882999999999996</v>
+      </c>
+      <c r="G22" t="s">
+        <v>9</v>
+      </c>
+      <c r="H22" t="s">
+        <v>9</v>
+      </c>
+      <c r="I22">
+        <v>78.179000000000002</v>
+      </c>
+      <c r="L22" t="s">
+        <v>29</v>
+      </c>
+      <c r="M22">
+        <v>2.8210000000000002</v>
+      </c>
+      <c r="N22">
+        <v>21.702999999999999</v>
+      </c>
+      <c r="O22">
+        <v>87.533000000000001</v>
+      </c>
+      <c r="P22" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>9</v>
+      </c>
+      <c r="R22">
+        <v>24.298999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>116</v>
+      </c>
+      <c r="C23" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" t="s">
+        <v>117</v>
+      </c>
+      <c r="E23" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" t="s">
+        <v>9</v>
+      </c>
+      <c r="G23" t="s">
+        <v>9</v>
+      </c>
+      <c r="H23" t="s">
+        <v>9</v>
+      </c>
+      <c r="I23" t="s">
+        <v>9</v>
+      </c>
+      <c r="K23" t="s">
+        <v>361</v>
+      </c>
+      <c r="L23" t="s">
+        <v>24</v>
+      </c>
+      <c r="M23" t="s">
+        <v>343</v>
+      </c>
+      <c r="N23" t="s">
+        <v>9</v>
+      </c>
+      <c r="O23" t="s">
+        <v>9</v>
+      </c>
+      <c r="P23" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>9</v>
+      </c>
+      <c r="R23" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="24" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C24" t="s">
+        <v>29</v>
+      </c>
+      <c r="D24">
+        <v>0.70899999999999996</v>
+      </c>
+      <c r="E24" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" t="s">
+        <v>9</v>
+      </c>
+      <c r="G24" t="s">
+        <v>9</v>
+      </c>
+      <c r="H24" t="s">
+        <v>9</v>
+      </c>
+      <c r="I24" t="s">
+        <v>9</v>
+      </c>
+      <c r="L24" t="s">
+        <v>29</v>
+      </c>
+      <c r="M24">
+        <v>1.254</v>
+      </c>
+      <c r="N24" t="s">
+        <v>9</v>
+      </c>
+      <c r="O24" t="s">
+        <v>9</v>
+      </c>
+      <c r="P24" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>9</v>
+      </c>
+      <c r="R24">
+        <v>42.055999999999997</v>
+      </c>
+    </row>
+    <row r="26" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B26" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="28" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" t="s">
+        <v>1</v>
+      </c>
+      <c r="D28" t="s">
+        <v>2</v>
+      </c>
+      <c r="E28" t="s">
+        <v>3</v>
+      </c>
+      <c r="F28" t="s">
+        <v>4</v>
+      </c>
+      <c r="G28" t="s">
+        <v>5</v>
+      </c>
+      <c r="H28" t="s">
+        <v>6</v>
+      </c>
+      <c r="I28" t="s">
+        <v>7</v>
+      </c>
+      <c r="K28" t="s">
+        <v>0</v>
+      </c>
+      <c r="L28" t="s">
+        <v>1</v>
+      </c>
+      <c r="M28" t="s">
+        <v>2</v>
+      </c>
+      <c r="N28" t="s">
+        <v>3</v>
+      </c>
+      <c r="O28" t="s">
+        <v>4</v>
+      </c>
+      <c r="P28" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>6</v>
+      </c>
+      <c r="R28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" t="s">
+        <v>24</v>
+      </c>
+      <c r="D29" t="s">
+        <v>25</v>
+      </c>
+      <c r="E29" t="s">
+        <v>26</v>
+      </c>
+      <c r="F29" t="s">
+        <v>27</v>
+      </c>
+      <c r="G29" t="s">
+        <v>28</v>
+      </c>
+      <c r="H29" t="s">
+        <v>9</v>
+      </c>
+      <c r="I29" t="s">
+        <v>9</v>
+      </c>
+      <c r="K29" t="s">
+        <v>175</v>
+      </c>
+      <c r="L29" t="s">
+        <v>24</v>
+      </c>
+      <c r="M29" t="s">
+        <v>176</v>
+      </c>
+      <c r="N29" t="s">
+        <v>9</v>
+      </c>
+      <c r="O29" t="s">
+        <v>177</v>
+      </c>
+      <c r="P29" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>9</v>
+      </c>
+      <c r="R29" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C30" t="s">
+        <v>29</v>
+      </c>
+      <c r="D30">
+        <v>0.09</v>
+      </c>
+      <c r="E30">
+        <v>67.328000000000003</v>
+      </c>
+      <c r="F30">
+        <v>0.434</v>
+      </c>
+      <c r="G30">
+        <v>2.57</v>
+      </c>
+      <c r="H30" t="s">
+        <v>9</v>
+      </c>
+      <c r="I30" t="s">
+        <v>9</v>
+      </c>
+      <c r="L30" t="s">
+        <v>29</v>
+      </c>
+      <c r="M30">
+        <v>0.312</v>
+      </c>
+      <c r="N30" t="s">
+        <v>9</v>
+      </c>
+      <c r="O30">
+        <v>11.813000000000001</v>
+      </c>
+      <c r="P30" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>9</v>
+      </c>
+      <c r="R30" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>10</v>
+      </c>
+      <c r="C31" t="s">
+        <v>24</v>
+      </c>
+      <c r="D31" t="s">
+        <v>30</v>
+      </c>
+      <c r="E31" t="s">
+        <v>9</v>
+      </c>
+      <c r="F31" t="s">
+        <v>31</v>
+      </c>
+      <c r="G31" t="s">
+        <v>32</v>
+      </c>
+      <c r="H31" t="s">
+        <v>33</v>
+      </c>
+      <c r="I31" t="s">
+        <v>9</v>
+      </c>
+      <c r="K31" t="s">
+        <v>178</v>
+      </c>
+      <c r="L31" t="s">
+        <v>24</v>
+      </c>
+      <c r="M31" t="s">
+        <v>179</v>
+      </c>
+      <c r="N31" t="s">
+        <v>9</v>
+      </c>
+      <c r="O31" t="s">
+        <v>9</v>
+      </c>
+      <c r="P31" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>9</v>
+      </c>
+      <c r="R31" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C32" t="s">
+        <v>29</v>
+      </c>
+      <c r="D32">
+        <v>0.18</v>
+      </c>
+      <c r="E32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32">
+        <v>1.054</v>
+      </c>
+      <c r="G32">
+        <v>1.2849999999999999</v>
+      </c>
+      <c r="H32">
+        <v>30.114000000000001</v>
+      </c>
+      <c r="I32" t="s">
+        <v>9</v>
+      </c>
+      <c r="L32" t="s">
+        <v>29</v>
+      </c>
+      <c r="M32">
+        <v>0.623</v>
+      </c>
+      <c r="N32" t="s">
+        <v>9</v>
+      </c>
+      <c r="O32" t="s">
+        <v>9</v>
+      </c>
+      <c r="P32" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>9</v>
+      </c>
+      <c r="R32" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" t="s">
+        <v>24</v>
+      </c>
+      <c r="D33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F33" t="s">
+        <v>35</v>
+      </c>
+      <c r="G33" t="s">
+        <v>36</v>
+      </c>
+      <c r="H33" t="s">
+        <v>37</v>
+      </c>
+      <c r="I33" t="s">
+        <v>9</v>
+      </c>
+      <c r="K33" t="s">
+        <v>196</v>
+      </c>
+      <c r="L33" t="s">
+        <v>24</v>
+      </c>
+      <c r="M33" t="s">
+        <v>197</v>
+      </c>
+      <c r="N33" t="s">
+        <v>9</v>
+      </c>
+      <c r="O33" t="s">
+        <v>9</v>
+      </c>
+      <c r="P33" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>9</v>
+      </c>
+      <c r="R33" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C34" t="s">
+        <v>29</v>
+      </c>
+      <c r="D34">
+        <v>0.27100000000000002</v>
+      </c>
+      <c r="E34" t="s">
+        <v>9</v>
+      </c>
+      <c r="F34">
+        <v>0.99199999999999999</v>
+      </c>
+      <c r="G34">
+        <v>2.9209999999999998</v>
+      </c>
+      <c r="H34">
+        <v>4.3559999999999999</v>
+      </c>
+      <c r="I34" t="s">
+        <v>9</v>
+      </c>
+      <c r="L34" t="s">
+        <v>29</v>
+      </c>
+      <c r="M34">
+        <v>0.93500000000000005</v>
+      </c>
+      <c r="N34" t="s">
+        <v>9</v>
+      </c>
+      <c r="O34" t="s">
+        <v>9</v>
+      </c>
+      <c r="P34">
+        <v>3.448</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>9</v>
+      </c>
+      <c r="R34" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35" t="s">
+        <v>24</v>
+      </c>
+      <c r="D35" t="s">
+        <v>38</v>
+      </c>
+      <c r="E35" t="s">
+        <v>39</v>
+      </c>
+      <c r="F35" t="s">
+        <v>40</v>
+      </c>
+      <c r="G35" t="s">
+        <v>41</v>
+      </c>
+      <c r="H35" t="s">
+        <v>42</v>
+      </c>
+      <c r="I35" t="s">
+        <v>9</v>
+      </c>
+      <c r="K35" t="s">
+        <v>199</v>
+      </c>
+      <c r="L35" t="s">
+        <v>24</v>
+      </c>
+      <c r="M35" t="s">
+        <v>197</v>
+      </c>
+      <c r="N35" t="s">
+        <v>9</v>
+      </c>
+      <c r="O35" t="s">
+        <v>9</v>
+      </c>
+      <c r="P35" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>9</v>
+      </c>
+      <c r="R35" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C36" t="s">
+        <v>29</v>
+      </c>
+      <c r="D36">
+        <v>0.36099999999999999</v>
+      </c>
+      <c r="E36">
+        <v>94.685000000000002</v>
+      </c>
+      <c r="F36">
+        <v>18.722999999999999</v>
+      </c>
+      <c r="G36">
+        <v>40.186999999999998</v>
+      </c>
+      <c r="H36">
+        <v>3.5979999999999999</v>
+      </c>
+      <c r="I36" t="s">
+        <v>9</v>
+      </c>
+      <c r="L36" t="s">
+        <v>29</v>
+      </c>
+      <c r="M36">
+        <v>0.93500000000000005</v>
+      </c>
+      <c r="N36" t="s">
+        <v>9</v>
+      </c>
+      <c r="O36" t="s">
+        <v>9</v>
+      </c>
+      <c r="P36">
+        <v>3.448</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>9</v>
+      </c>
+      <c r="R36" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
+        <v>13</v>
+      </c>
+      <c r="C37" t="s">
+        <v>24</v>
+      </c>
+      <c r="D37" t="s">
+        <v>43</v>
+      </c>
+      <c r="E37" t="s">
+        <v>44</v>
+      </c>
+      <c r="F37" t="s">
+        <v>9</v>
+      </c>
+      <c r="G37" t="s">
+        <v>45</v>
+      </c>
+      <c r="H37" t="s">
+        <v>46</v>
+      </c>
+      <c r="I37" t="s">
+        <v>9</v>
+      </c>
+      <c r="K37" t="s">
+        <v>362</v>
+      </c>
+      <c r="L37" t="s">
+        <v>24</v>
+      </c>
+      <c r="M37" t="s">
+        <v>363</v>
+      </c>
+      <c r="N37" t="s">
+        <v>9</v>
+      </c>
+      <c r="O37" t="s">
+        <v>9</v>
+      </c>
+      <c r="P37" t="s">
+        <v>364</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>9</v>
+      </c>
+      <c r="R37" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C38" t="s">
+        <v>29</v>
+      </c>
+      <c r="D38">
+        <v>0.45100000000000001</v>
+      </c>
+      <c r="E38">
+        <v>53.295999999999999</v>
+      </c>
+      <c r="F38" t="s">
+        <v>9</v>
+      </c>
+      <c r="G38">
+        <v>5.9580000000000002</v>
+      </c>
+      <c r="H38">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="I38" t="s">
+        <v>9</v>
+      </c>
+      <c r="L38" t="s">
+        <v>29</v>
+      </c>
+      <c r="M38">
+        <v>1.5580000000000001</v>
+      </c>
+      <c r="N38" t="s">
+        <v>9</v>
+      </c>
+      <c r="O38" t="s">
+        <v>9</v>
+      </c>
+      <c r="P38">
+        <v>4.5090000000000003</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>9</v>
+      </c>
+      <c r="R38" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39" t="s">
+        <v>24</v>
+      </c>
+      <c r="D39" t="s">
+        <v>47</v>
+      </c>
+      <c r="E39" t="s">
+        <v>9</v>
+      </c>
+      <c r="F39" t="s">
+        <v>48</v>
+      </c>
+      <c r="G39" t="s">
+        <v>49</v>
+      </c>
+      <c r="H39" t="s">
+        <v>9</v>
+      </c>
+      <c r="I39" t="s">
+        <v>9</v>
+      </c>
+      <c r="K39" t="s">
+        <v>324</v>
+      </c>
+      <c r="L39" t="s">
+        <v>24</v>
+      </c>
+      <c r="M39" t="s">
+        <v>327</v>
+      </c>
+      <c r="N39" t="s">
+        <v>9</v>
+      </c>
+      <c r="O39" t="s">
+        <v>9</v>
+      </c>
+      <c r="P39" t="s">
+        <v>326</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>325</v>
+      </c>
+      <c r="R39" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C40" t="s">
+        <v>29</v>
+      </c>
+      <c r="D40">
+        <v>0.54100000000000004</v>
+      </c>
+      <c r="E40" t="s">
+        <v>9</v>
+      </c>
+      <c r="F40">
+        <v>2.17</v>
+      </c>
+      <c r="G40">
+        <v>2.6869999999999998</v>
+      </c>
+      <c r="H40" t="s">
+        <v>9</v>
+      </c>
+      <c r="I40" t="s">
+        <v>9</v>
+      </c>
+      <c r="L40" t="s">
+        <v>29</v>
+      </c>
+      <c r="M40">
+        <v>1.869</v>
+      </c>
+      <c r="N40" t="s">
+        <v>9</v>
+      </c>
+      <c r="O40" t="s">
+        <v>9</v>
+      </c>
+      <c r="P40">
+        <v>2.387</v>
+      </c>
+      <c r="Q40">
+        <v>1.133</v>
+      </c>
+      <c r="R40" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
+        <v>15</v>
+      </c>
+      <c r="C41" t="s">
+        <v>24</v>
+      </c>
+      <c r="D41" t="s">
+        <v>50</v>
+      </c>
+      <c r="E41" t="s">
+        <v>9</v>
+      </c>
+      <c r="F41" t="s">
+        <v>51</v>
+      </c>
+      <c r="G41" t="s">
+        <v>52</v>
+      </c>
+      <c r="H41" t="s">
+        <v>9</v>
+      </c>
+      <c r="I41" t="s">
+        <v>9</v>
+      </c>
+      <c r="K41" t="s">
+        <v>365</v>
+      </c>
+      <c r="L41" t="s">
+        <v>24</v>
+      </c>
+      <c r="M41" t="s">
+        <v>366</v>
+      </c>
+      <c r="N41" t="s">
+        <v>367</v>
+      </c>
+      <c r="O41" t="s">
+        <v>368</v>
+      </c>
+      <c r="P41" t="s">
+        <v>369</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>9</v>
+      </c>
+      <c r="R41" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C42" t="s">
+        <v>29</v>
+      </c>
+      <c r="D42">
+        <v>0.63100000000000001</v>
+      </c>
+      <c r="E42" t="s">
+        <v>9</v>
+      </c>
+      <c r="F42">
+        <v>0.496</v>
+      </c>
+      <c r="G42">
+        <v>1.986</v>
+      </c>
+      <c r="H42" t="s">
+        <v>9</v>
+      </c>
+      <c r="I42" t="s">
+        <v>9</v>
+      </c>
+      <c r="L42" t="s">
+        <v>29</v>
+      </c>
+      <c r="M42">
+        <v>2.181</v>
+      </c>
+      <c r="N42">
+        <v>90.281999999999996</v>
+      </c>
+      <c r="O42">
+        <v>9.0660000000000007</v>
+      </c>
+      <c r="P42">
+        <v>5.57</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>9</v>
+      </c>
+      <c r="R42" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
+        <v>16</v>
+      </c>
+      <c r="C43" t="s">
+        <v>24</v>
+      </c>
+      <c r="D43" t="s">
+        <v>53</v>
+      </c>
+      <c r="E43" t="s">
+        <v>54</v>
+      </c>
+      <c r="F43" t="s">
+        <v>55</v>
+      </c>
+      <c r="G43" t="s">
+        <v>56</v>
+      </c>
+      <c r="H43" t="s">
+        <v>9</v>
+      </c>
+      <c r="I43" t="s">
+        <v>9</v>
+      </c>
+      <c r="K43" t="s">
+        <v>262</v>
+      </c>
+      <c r="L43" t="s">
+        <v>24</v>
+      </c>
+      <c r="M43" t="s">
+        <v>338</v>
+      </c>
+      <c r="N43" t="s">
+        <v>335</v>
+      </c>
+      <c r="O43" t="s">
+        <v>336</v>
+      </c>
+      <c r="P43" t="s">
+        <v>337</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>334</v>
+      </c>
+      <c r="R43" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="44" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C44" t="s">
+        <v>29</v>
+      </c>
+      <c r="D44">
+        <v>0.72099999999999997</v>
+      </c>
+      <c r="E44">
+        <v>19.347999999999999</v>
+      </c>
+      <c r="F44">
+        <v>3.3479999999999999</v>
+      </c>
+      <c r="G44">
+        <v>42.173000000000002</v>
+      </c>
+      <c r="H44" t="s">
+        <v>9</v>
+      </c>
+      <c r="I44" t="s">
+        <v>9</v>
+      </c>
+      <c r="L44" t="s">
+        <v>29</v>
+      </c>
+      <c r="M44">
+        <v>2.492</v>
+      </c>
+      <c r="N44">
+        <v>11.599</v>
+      </c>
+      <c r="O44">
+        <v>8.2420000000000009</v>
+      </c>
+      <c r="P44">
+        <v>6.101</v>
+      </c>
+      <c r="Q44">
+        <v>1.456</v>
+      </c>
+      <c r="R44">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="45" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
+        <v>17</v>
+      </c>
+      <c r="C45" t="s">
+        <v>24</v>
+      </c>
+      <c r="D45" t="s">
+        <v>57</v>
+      </c>
+      <c r="E45" t="s">
+        <v>58</v>
+      </c>
+      <c r="F45" t="s">
+        <v>59</v>
+      </c>
+      <c r="G45" t="s">
+        <v>60</v>
+      </c>
+      <c r="H45" t="s">
+        <v>61</v>
+      </c>
+      <c r="I45" t="s">
+        <v>9</v>
+      </c>
+      <c r="K45" t="s">
+        <v>371</v>
+      </c>
+      <c r="L45" t="s">
+        <v>24</v>
+      </c>
+      <c r="M45" t="s">
+        <v>372</v>
+      </c>
+      <c r="N45" t="s">
+        <v>373</v>
+      </c>
+      <c r="O45" t="s">
+        <v>374</v>
+      </c>
+      <c r="P45" t="s">
+        <v>375</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>9</v>
+      </c>
+      <c r="R45" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C46" t="s">
+        <v>29</v>
+      </c>
+      <c r="D46">
+        <v>0.81200000000000006</v>
+      </c>
+      <c r="E46">
+        <v>1.276</v>
+      </c>
+      <c r="F46">
+        <v>1.984</v>
+      </c>
+      <c r="G46">
+        <v>7.593</v>
+      </c>
+      <c r="H46">
+        <v>13.446999999999999</v>
+      </c>
+      <c r="I46" t="s">
+        <v>9</v>
+      </c>
+      <c r="L46" t="s">
+        <v>29</v>
+      </c>
+      <c r="M46">
+        <v>2.8039999999999998</v>
+      </c>
+      <c r="N46">
+        <v>59.875</v>
+      </c>
+      <c r="O46">
+        <v>14.286</v>
+      </c>
+      <c r="P46">
+        <v>7.4269999999999996</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>9</v>
+      </c>
+      <c r="R46" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B47" t="s">
+        <v>18</v>
+      </c>
+      <c r="C47" t="s">
+        <v>24</v>
+      </c>
+      <c r="D47" t="s">
+        <v>62</v>
+      </c>
+      <c r="E47" t="s">
+        <v>9</v>
+      </c>
+      <c r="F47" t="s">
+        <v>63</v>
+      </c>
+      <c r="G47" t="s">
+        <v>64</v>
+      </c>
+      <c r="H47" t="s">
+        <v>9</v>
+      </c>
+      <c r="I47" t="s">
+        <v>9</v>
+      </c>
+      <c r="K47" t="s">
+        <v>376</v>
+      </c>
+      <c r="L47" t="s">
+        <v>24</v>
+      </c>
+      <c r="M47" t="s">
+        <v>377</v>
+      </c>
+      <c r="N47" t="s">
+        <v>378</v>
+      </c>
+      <c r="O47" t="s">
+        <v>379</v>
+      </c>
+      <c r="P47" t="s">
+        <v>380</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>9</v>
+      </c>
+      <c r="R47" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C48" t="s">
+        <v>29</v>
+      </c>
+      <c r="D48">
+        <v>0.90200000000000002</v>
+      </c>
+      <c r="E48" t="s">
+        <v>9</v>
+      </c>
+      <c r="F48">
+        <v>55.115000000000002</v>
+      </c>
+      <c r="G48">
+        <v>10.164</v>
+      </c>
+      <c r="H48" t="s">
+        <v>9</v>
+      </c>
+      <c r="I48" t="s">
+        <v>9</v>
+      </c>
+      <c r="L48" t="s">
+        <v>29</v>
+      </c>
+      <c r="M48">
+        <v>3.1150000000000002</v>
+      </c>
+      <c r="N48">
+        <v>85.58</v>
+      </c>
+      <c r="O48">
+        <v>56.319000000000003</v>
+      </c>
+      <c r="P48">
+        <v>19.097999999999999</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>9</v>
+      </c>
+      <c r="R48" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B49" t="s">
+        <v>19</v>
+      </c>
+      <c r="C49" t="s">
+        <v>24</v>
+      </c>
+      <c r="D49" t="s">
+        <v>62</v>
+      </c>
+      <c r="E49" t="s">
+        <v>26</v>
+      </c>
+      <c r="F49" t="s">
+        <v>26</v>
+      </c>
+      <c r="G49" t="s">
+        <v>65</v>
+      </c>
+      <c r="H49" t="s">
+        <v>9</v>
+      </c>
+      <c r="I49" t="s">
+        <v>9</v>
+      </c>
+      <c r="K49" t="s">
+        <v>295</v>
+      </c>
+      <c r="L49" t="s">
+        <v>24</v>
+      </c>
+      <c r="M49" t="s">
+        <v>300</v>
+      </c>
+      <c r="N49" t="s">
+        <v>297</v>
+      </c>
+      <c r="O49" t="s">
+        <v>298</v>
+      </c>
+      <c r="P49" t="s">
+        <v>381</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>296</v>
+      </c>
+      <c r="R49" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="50" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C50" t="s">
+        <v>29</v>
+      </c>
+      <c r="D50">
+        <v>0.99199999999999999</v>
+      </c>
+      <c r="E50">
+        <v>68.037000000000006</v>
+      </c>
+      <c r="F50">
+        <v>79.230999999999995</v>
+      </c>
+      <c r="G50">
+        <v>8.4109999999999996</v>
+      </c>
+      <c r="H50" t="s">
+        <v>9</v>
+      </c>
+      <c r="I50" t="s">
+        <v>9</v>
+      </c>
+      <c r="L50" t="s">
+        <v>29</v>
+      </c>
+      <c r="M50">
+        <v>3.427</v>
+      </c>
+      <c r="N50">
+        <v>88.400999999999996</v>
+      </c>
+      <c r="O50">
+        <v>41.484000000000002</v>
+      </c>
+      <c r="P50">
+        <v>7.9580000000000002</v>
+      </c>
+      <c r="Q50">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="R50">
+        <v>13.333</v>
+      </c>
+    </row>
+    <row r="51" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B51" t="s">
+        <v>20</v>
+      </c>
+      <c r="C51" t="s">
+        <v>24</v>
+      </c>
+      <c r="D51" t="s">
+        <v>48</v>
+      </c>
+      <c r="E51" t="s">
+        <v>66</v>
+      </c>
+      <c r="F51" t="s">
+        <v>67</v>
+      </c>
+      <c r="G51" t="s">
+        <v>68</v>
+      </c>
+      <c r="H51" t="s">
+        <v>9</v>
+      </c>
+      <c r="I51" t="s">
+        <v>9</v>
+      </c>
+      <c r="K51" t="s">
+        <v>383</v>
+      </c>
+      <c r="L51" t="s">
+        <v>24</v>
+      </c>
+      <c r="M51" t="s">
+        <v>384</v>
+      </c>
+      <c r="N51" t="s">
+        <v>9</v>
+      </c>
+      <c r="O51" t="s">
+        <v>385</v>
+      </c>
+      <c r="P51" t="s">
+        <v>386</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>9</v>
+      </c>
+      <c r="R51" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C52" t="s">
+        <v>29</v>
+      </c>
+      <c r="D52">
+        <v>1.0820000000000001</v>
+      </c>
+      <c r="E52">
+        <v>2.5510000000000002</v>
+      </c>
+      <c r="F52">
+        <v>11.035</v>
+      </c>
+      <c r="G52">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="H52" t="s">
+        <v>9</v>
+      </c>
+      <c r="I52" t="s">
+        <v>9</v>
+      </c>
+      <c r="L52" t="s">
+        <v>29</v>
+      </c>
+      <c r="M52">
+        <v>3.738</v>
+      </c>
+      <c r="N52" t="s">
+        <v>9</v>
+      </c>
+      <c r="O52">
+        <v>94.78</v>
+      </c>
+      <c r="P52">
+        <v>88.328999999999994</v>
+      </c>
+      <c r="Q52" t="s">
+        <v>9</v>
+      </c>
+      <c r="R52" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="53" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B53" t="s">
+        <v>21</v>
+      </c>
+      <c r="C53" t="s">
+        <v>24</v>
+      </c>
+      <c r="D53" t="s">
+        <v>69</v>
+      </c>
+      <c r="E53" t="s">
+        <v>9</v>
+      </c>
+      <c r="F53" t="s">
+        <v>9</v>
+      </c>
+      <c r="G53" t="s">
+        <v>9</v>
+      </c>
+      <c r="H53" t="s">
+        <v>70</v>
+      </c>
+      <c r="I53" t="s">
+        <v>9</v>
+      </c>
+      <c r="K53" t="s">
+        <v>387</v>
+      </c>
+      <c r="L53" t="s">
+        <v>24</v>
+      </c>
+      <c r="M53" t="s">
+        <v>388</v>
+      </c>
+      <c r="N53" t="s">
+        <v>9</v>
+      </c>
+      <c r="O53" t="s">
+        <v>9</v>
+      </c>
+      <c r="P53" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q53" t="s">
+        <v>9</v>
+      </c>
+      <c r="R53" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C54" t="s">
+        <v>29</v>
+      </c>
+      <c r="D54">
+        <v>1.1719999999999999</v>
+      </c>
+      <c r="E54" t="s">
+        <v>9</v>
+      </c>
+      <c r="F54" t="s">
+        <v>9</v>
+      </c>
+      <c r="G54" t="s">
+        <v>9</v>
+      </c>
+      <c r="H54">
+        <v>20.928000000000001</v>
+      </c>
+      <c r="I54" t="s">
+        <v>9</v>
+      </c>
+      <c r="L54" t="s">
+        <v>29</v>
+      </c>
+      <c r="M54">
+        <v>4.05</v>
+      </c>
+      <c r="N54" t="s">
+        <v>9</v>
+      </c>
+      <c r="O54" t="s">
+        <v>9</v>
+      </c>
+      <c r="P54" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q54" t="s">
+        <v>9</v>
+      </c>
+      <c r="R54" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B55" t="s">
+        <v>22</v>
+      </c>
+      <c r="C55" t="s">
+        <v>24</v>
+      </c>
+      <c r="D55" t="s">
+        <v>71</v>
+      </c>
+      <c r="E55" t="s">
+        <v>72</v>
+      </c>
+      <c r="F55" t="s">
+        <v>73</v>
+      </c>
+      <c r="G55" t="s">
+        <v>74</v>
+      </c>
+      <c r="H55" t="s">
+        <v>75</v>
+      </c>
+      <c r="I55" t="s">
+        <v>76</v>
+      </c>
+      <c r="K55" t="s">
+        <v>328</v>
+      </c>
+      <c r="L55" t="s">
+        <v>24</v>
+      </c>
+      <c r="M55" t="s">
+        <v>333</v>
+      </c>
+      <c r="N55" t="s">
+        <v>330</v>
+      </c>
+      <c r="O55" t="s">
+        <v>331</v>
+      </c>
+      <c r="P55" t="s">
+        <v>332</v>
+      </c>
+      <c r="Q55" t="s">
+        <v>329</v>
+      </c>
+      <c r="R55" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="56" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C56" t="s">
+        <v>29</v>
+      </c>
+      <c r="D56">
+        <v>1.262</v>
+      </c>
+      <c r="E56">
+        <v>82.849000000000004</v>
+      </c>
+      <c r="F56">
+        <v>19.963000000000001</v>
+      </c>
+      <c r="G56">
+        <v>7.4770000000000003</v>
+      </c>
+      <c r="H56">
+        <v>5.0190000000000001</v>
+      </c>
+      <c r="I56">
+        <v>2.3210000000000002</v>
+      </c>
+      <c r="L56" t="s">
+        <v>29</v>
+      </c>
+      <c r="M56">
+        <v>4.3609999999999998</v>
+      </c>
+      <c r="N56">
+        <v>20.376000000000001</v>
+      </c>
+      <c r="O56">
+        <v>8.516</v>
+      </c>
+      <c r="P56">
+        <v>9.0190000000000001</v>
+      </c>
+      <c r="Q56">
+        <v>1.294</v>
+      </c>
+      <c r="R56" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="57" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B57" t="s">
+        <v>23</v>
+      </c>
+      <c r="C57" t="s">
+        <v>24</v>
+      </c>
+      <c r="D57" t="s">
+        <v>77</v>
+      </c>
+      <c r="E57" t="s">
+        <v>78</v>
+      </c>
+      <c r="F57" t="s">
+        <v>79</v>
+      </c>
+      <c r="G57" t="s">
+        <v>80</v>
+      </c>
+      <c r="H57" t="s">
+        <v>81</v>
+      </c>
+      <c r="I57" t="s">
+        <v>82</v>
+      </c>
+      <c r="K57" t="s">
+        <v>389</v>
+      </c>
+      <c r="L57" t="s">
+        <v>24</v>
+      </c>
+      <c r="M57" t="s">
+        <v>390</v>
+      </c>
+      <c r="N57" t="s">
+        <v>391</v>
+      </c>
+      <c r="O57" t="s">
+        <v>392</v>
+      </c>
+      <c r="P57" t="s">
+        <v>393</v>
+      </c>
+      <c r="Q57" t="s">
+        <v>9</v>
+      </c>
+      <c r="R57" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="58" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C58" t="s">
+        <v>29</v>
+      </c>
+      <c r="D58">
+        <v>1.353</v>
+      </c>
+      <c r="E58">
+        <v>37.066000000000003</v>
+      </c>
+      <c r="F58">
+        <v>43.954999999999998</v>
+      </c>
+      <c r="G58">
+        <v>59.695999999999998</v>
+      </c>
+      <c r="H58">
+        <v>15.72</v>
+      </c>
+      <c r="I58">
+        <v>54.219000000000001</v>
+      </c>
+      <c r="L58" t="s">
+        <v>29</v>
+      </c>
+      <c r="M58">
+        <v>4.673</v>
+      </c>
+      <c r="N58">
+        <v>10.031000000000001</v>
+      </c>
+      <c r="O58">
+        <v>10.44</v>
+      </c>
+      <c r="P58">
+        <v>12.202</v>
+      </c>
+      <c r="Q58" t="s">
+        <v>9</v>
+      </c>
+      <c r="R58" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="60" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B60" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="61" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B61" t="s">
+        <v>0</v>
+      </c>
+      <c r="C61" t="s">
+        <v>1</v>
+      </c>
+      <c r="D61" t="s">
+        <v>5</v>
+      </c>
+      <c r="E61" t="s">
+        <v>3</v>
+      </c>
+      <c r="F61" t="s">
+        <v>4</v>
+      </c>
+      <c r="G61" t="s">
+        <v>6</v>
+      </c>
+      <c r="H61" t="s">
+        <v>7</v>
+      </c>
+      <c r="I61" t="s">
+        <v>2</v>
+      </c>
+      <c r="K61" t="s">
+        <v>0</v>
+      </c>
+      <c r="L61" t="s">
+        <v>1</v>
+      </c>
+      <c r="M61" t="s">
+        <v>5</v>
+      </c>
+      <c r="N61" t="s">
+        <v>3</v>
+      </c>
+      <c r="O61" t="s">
+        <v>4</v>
+      </c>
+      <c r="P61" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q61" t="s">
+        <v>7</v>
+      </c>
+      <c r="R61" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B62" t="s">
+        <v>212</v>
+      </c>
+      <c r="C62" t="s">
+        <v>24</v>
+      </c>
+      <c r="D62" t="s">
+        <v>213</v>
+      </c>
+      <c r="E62" t="s">
+        <v>9</v>
+      </c>
+      <c r="F62" t="s">
+        <v>9</v>
+      </c>
+      <c r="G62" t="s">
+        <v>9</v>
+      </c>
+      <c r="H62" t="s">
+        <v>9</v>
+      </c>
+      <c r="I62" t="s">
+        <v>9</v>
+      </c>
+      <c r="K62" t="s">
+        <v>238</v>
+      </c>
+      <c r="L62" t="s">
+        <v>24</v>
+      </c>
+      <c r="M62" t="s">
+        <v>239</v>
+      </c>
+      <c r="N62" t="s">
+        <v>9</v>
+      </c>
+      <c r="O62" t="s">
+        <v>9</v>
+      </c>
+      <c r="P62" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q62" t="s">
+        <v>9</v>
+      </c>
+      <c r="R62" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="63" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C63" t="s">
+        <v>29</v>
+      </c>
+      <c r="D63">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="E63" t="s">
+        <v>9</v>
+      </c>
+      <c r="F63" t="s">
+        <v>9</v>
+      </c>
+      <c r="G63" t="s">
+        <v>9</v>
+      </c>
+      <c r="H63" t="s">
+        <v>9</v>
+      </c>
+      <c r="I63" t="s">
+        <v>9</v>
+      </c>
+      <c r="L63" t="s">
+        <v>29</v>
+      </c>
+      <c r="M63">
+        <v>0.18099999999999999</v>
+      </c>
+      <c r="N63" t="s">
+        <v>9</v>
+      </c>
+      <c r="O63" t="s">
+        <v>9</v>
+      </c>
+      <c r="P63" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q63" t="s">
+        <v>9</v>
+      </c>
+      <c r="R63">
+        <v>6.6820000000000004</v>
+      </c>
+    </row>
+    <row r="64" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B64" t="s">
+        <v>214</v>
+      </c>
+      <c r="C64" t="s">
+        <v>24</v>
+      </c>
+      <c r="D64" t="s">
+        <v>213</v>
+      </c>
+      <c r="E64" t="s">
+        <v>9</v>
+      </c>
+      <c r="F64" t="s">
+        <v>9</v>
+      </c>
+      <c r="G64" t="s">
+        <v>9</v>
+      </c>
+      <c r="H64" t="s">
+        <v>9</v>
+      </c>
+      <c r="I64" t="s">
+        <v>9</v>
+      </c>
+      <c r="K64" t="s">
+        <v>241</v>
+      </c>
+      <c r="L64" t="s">
+        <v>24</v>
+      </c>
+      <c r="M64" t="s">
+        <v>242</v>
+      </c>
+      <c r="N64" t="s">
+        <v>243</v>
+      </c>
+      <c r="O64" t="s">
+        <v>9</v>
+      </c>
+      <c r="P64" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q64" t="s">
+        <v>9</v>
+      </c>
+      <c r="R64" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="65" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C65" t="s">
+        <v>29</v>
+      </c>
+      <c r="D65">
+        <v>0.23400000000000001</v>
+      </c>
+      <c r="E65" t="s">
+        <v>9</v>
+      </c>
+      <c r="F65" t="s">
+        <v>9</v>
+      </c>
+      <c r="G65" t="s">
+        <v>9</v>
+      </c>
+      <c r="H65" t="s">
+        <v>9</v>
+      </c>
+      <c r="I65" t="s">
+        <v>9</v>
+      </c>
+      <c r="L65" t="s">
+        <v>29</v>
+      </c>
+      <c r="M65">
+        <v>0.36199999999999999</v>
+      </c>
+      <c r="N65">
+        <v>6.8739999999999997</v>
+      </c>
+      <c r="O65" t="s">
+        <v>9</v>
+      </c>
+      <c r="P65" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q65" t="s">
+        <v>9</v>
+      </c>
+      <c r="R65" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="66" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B66" t="s">
+        <v>215</v>
+      </c>
+      <c r="C66" t="s">
+        <v>24</v>
+      </c>
+      <c r="D66" t="s">
+        <v>216</v>
+      </c>
+      <c r="E66" t="s">
+        <v>26</v>
+      </c>
+      <c r="F66" t="s">
+        <v>26</v>
+      </c>
+      <c r="G66" t="s">
+        <v>70</v>
+      </c>
+      <c r="H66" t="s">
+        <v>9</v>
+      </c>
+      <c r="I66" t="s">
+        <v>217</v>
+      </c>
+      <c r="K66" t="s">
+        <v>244</v>
+      </c>
+      <c r="L66" t="s">
+        <v>24</v>
+      </c>
+      <c r="M66" t="s">
+        <v>245</v>
+      </c>
+      <c r="N66" t="s">
+        <v>9</v>
+      </c>
+      <c r="O66" t="s">
+        <v>246</v>
+      </c>
+      <c r="P66" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q66" t="s">
+        <v>9</v>
+      </c>
+      <c r="R66" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="67" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C67" t="s">
+        <v>29</v>
+      </c>
+      <c r="D67">
+        <v>0.35</v>
+      </c>
+      <c r="E67">
+        <v>62.509</v>
+      </c>
+      <c r="F67">
+        <v>75.635000000000005</v>
+      </c>
+      <c r="G67">
+        <v>18.939</v>
+      </c>
+      <c r="H67" t="s">
+        <v>9</v>
+      </c>
+      <c r="I67">
+        <v>1.4430000000000001</v>
+      </c>
+      <c r="L67" t="s">
+        <v>29</v>
+      </c>
+      <c r="M67">
+        <v>0.54300000000000004</v>
+      </c>
+      <c r="N67" t="s">
+        <v>9</v>
+      </c>
+      <c r="O67">
+        <v>8.6709999999999994</v>
+      </c>
+      <c r="P67" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q67" t="s">
+        <v>9</v>
+      </c>
+      <c r="R67" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="68" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B68" t="s">
+        <v>218</v>
+      </c>
+      <c r="C68" t="s">
+        <v>24</v>
+      </c>
+      <c r="D68" t="s">
+        <v>219</v>
+      </c>
+      <c r="E68" t="s">
+        <v>9</v>
+      </c>
+      <c r="F68" t="s">
+        <v>220</v>
+      </c>
+      <c r="G68" t="s">
+        <v>221</v>
+      </c>
+      <c r="H68" t="s">
+        <v>9</v>
+      </c>
+      <c r="I68" t="s">
+        <v>222</v>
+      </c>
+      <c r="K68" t="s">
+        <v>247</v>
+      </c>
+      <c r="L68" t="s">
+        <v>24</v>
+      </c>
+      <c r="M68" t="s">
+        <v>245</v>
+      </c>
+      <c r="N68" t="s">
+        <v>9</v>
+      </c>
+      <c r="O68" t="s">
+        <v>248</v>
+      </c>
+      <c r="P68" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q68" t="s">
+        <v>9</v>
+      </c>
+      <c r="R68" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="69" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C69" t="s">
+        <v>29</v>
+      </c>
+      <c r="D69">
+        <v>0.46700000000000003</v>
+      </c>
+      <c r="E69" t="s">
+        <v>9</v>
+      </c>
+      <c r="F69">
+        <v>10.353</v>
+      </c>
+      <c r="G69">
+        <v>53.597999999999999</v>
+      </c>
+      <c r="H69" t="s">
+        <v>9</v>
+      </c>
+      <c r="I69">
+        <v>13.885999999999999</v>
+      </c>
+      <c r="L69" t="s">
+        <v>29</v>
+      </c>
+      <c r="M69">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="N69" t="s">
+        <v>9</v>
+      </c>
+      <c r="O69">
+        <v>8.4779999999999998</v>
+      </c>
+      <c r="P69" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q69" t="s">
+        <v>9</v>
+      </c>
+      <c r="R69" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="70" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B70" t="s">
+        <v>223</v>
+      </c>
+      <c r="C70" t="s">
+        <v>24</v>
+      </c>
+      <c r="D70" t="s">
+        <v>224</v>
+      </c>
+      <c r="E70" t="s">
+        <v>9</v>
+      </c>
+      <c r="F70" t="s">
+        <v>9</v>
+      </c>
+      <c r="G70" t="s">
+        <v>9</v>
+      </c>
+      <c r="H70" t="s">
+        <v>9</v>
+      </c>
+      <c r="I70" t="s">
+        <v>9</v>
+      </c>
+      <c r="K70" t="s">
+        <v>249</v>
+      </c>
+      <c r="L70" t="s">
+        <v>24</v>
+      </c>
+      <c r="M70" t="s">
+        <v>250</v>
+      </c>
+      <c r="N70" t="s">
+        <v>9</v>
+      </c>
+      <c r="O70" t="s">
+        <v>179</v>
+      </c>
+      <c r="P70" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q70" t="s">
+        <v>9</v>
+      </c>
+      <c r="R70" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="71" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C71" t="s">
+        <v>29</v>
+      </c>
+      <c r="D71">
+        <v>0.58399999999999996</v>
+      </c>
+      <c r="E71" t="s">
+        <v>9</v>
+      </c>
+      <c r="F71" t="s">
+        <v>9</v>
+      </c>
+      <c r="G71" t="s">
+        <v>9</v>
+      </c>
+      <c r="H71" t="s">
+        <v>9</v>
+      </c>
+      <c r="I71" t="s">
+        <v>9</v>
+      </c>
+      <c r="L71" t="s">
+        <v>29</v>
+      </c>
+      <c r="M71">
+        <v>0.90600000000000003</v>
+      </c>
+      <c r="N71" t="s">
+        <v>9</v>
+      </c>
+      <c r="O71">
+        <v>4.8170000000000002</v>
+      </c>
+      <c r="P71" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q71" t="s">
+        <v>9</v>
+      </c>
+      <c r="R71" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="72" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B72" t="s">
+        <v>225</v>
+      </c>
+      <c r="C72" t="s">
+        <v>24</v>
+      </c>
+      <c r="D72" t="s">
+        <v>226</v>
+      </c>
+      <c r="E72" t="s">
+        <v>9</v>
+      </c>
+      <c r="F72" t="s">
+        <v>9</v>
+      </c>
+      <c r="G72" t="s">
+        <v>9</v>
+      </c>
+      <c r="H72" t="s">
+        <v>9</v>
+      </c>
+      <c r="I72" t="s">
+        <v>9</v>
+      </c>
+      <c r="K72" t="s">
+        <v>251</v>
+      </c>
+      <c r="L72" t="s">
+        <v>24</v>
+      </c>
+      <c r="M72" t="s">
+        <v>245</v>
+      </c>
+      <c r="N72" t="s">
+        <v>9</v>
+      </c>
+      <c r="O72" t="s">
+        <v>248</v>
+      </c>
+      <c r="P72" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q72" t="s">
+        <v>9</v>
+      </c>
+      <c r="R72" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="73" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C73" t="s">
+        <v>29</v>
+      </c>
+      <c r="D73">
+        <v>0.70099999999999996</v>
+      </c>
+      <c r="E73" t="s">
+        <v>9</v>
+      </c>
+      <c r="F73" t="s">
+        <v>9</v>
+      </c>
+      <c r="G73" t="s">
+        <v>9</v>
+      </c>
+      <c r="H73" t="s">
+        <v>9</v>
+      </c>
+      <c r="I73" t="s">
+        <v>9</v>
+      </c>
+      <c r="L73" t="s">
+        <v>29</v>
+      </c>
+      <c r="M73">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="N73" t="s">
+        <v>9</v>
+      </c>
+      <c r="O73">
+        <v>8.4779999999999998</v>
+      </c>
+      <c r="P73" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q73" t="s">
+        <v>9</v>
+      </c>
+      <c r="R73" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="74" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B74" t="s">
+        <v>227</v>
+      </c>
+      <c r="C74" t="s">
+        <v>24</v>
+      </c>
+      <c r="D74" t="s">
+        <v>228</v>
+      </c>
+      <c r="E74" t="s">
+        <v>113</v>
+      </c>
+      <c r="F74" t="s">
+        <v>9</v>
+      </c>
+      <c r="G74" t="s">
+        <v>9</v>
+      </c>
+      <c r="H74" t="s">
+        <v>9</v>
+      </c>
+      <c r="I74" t="s">
+        <v>9</v>
+      </c>
+      <c r="K74" t="s">
+        <v>252</v>
+      </c>
+      <c r="L74" t="s">
+        <v>24</v>
+      </c>
+      <c r="M74" t="s">
+        <v>253</v>
+      </c>
+      <c r="N74" t="s">
+        <v>9</v>
+      </c>
+      <c r="O74" t="s">
+        <v>187</v>
+      </c>
+      <c r="P74" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q74" t="s">
+        <v>9</v>
+      </c>
+      <c r="R74" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="75" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C75" t="s">
+        <v>29</v>
+      </c>
+      <c r="D75">
+        <v>0.81799999999999995</v>
+      </c>
+      <c r="E75">
+        <v>32.317999999999998</v>
+      </c>
+      <c r="F75" t="s">
+        <v>9</v>
+      </c>
+      <c r="G75" t="s">
+        <v>9</v>
+      </c>
+      <c r="H75" t="s">
+        <v>9</v>
+      </c>
+      <c r="I75" t="s">
+        <v>9</v>
+      </c>
+      <c r="L75" t="s">
+        <v>29</v>
+      </c>
+      <c r="M75">
+        <v>1.268</v>
+      </c>
+      <c r="N75" t="s">
+        <v>9</v>
+      </c>
+      <c r="O75">
+        <v>3.0830000000000002</v>
+      </c>
+      <c r="P75" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q75" t="s">
+        <v>9</v>
+      </c>
+      <c r="R75" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="76" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B76" t="s">
+        <v>229</v>
+      </c>
+      <c r="C76" t="s">
+        <v>24</v>
+      </c>
+      <c r="D76" t="s">
+        <v>230</v>
+      </c>
+      <c r="E76" t="s">
+        <v>9</v>
+      </c>
+      <c r="F76" t="s">
+        <v>231</v>
+      </c>
+      <c r="G76" t="s">
+        <v>9</v>
+      </c>
+      <c r="H76" t="s">
+        <v>9</v>
+      </c>
+      <c r="I76" t="s">
+        <v>9</v>
+      </c>
+      <c r="K76" t="s">
+        <v>204</v>
+      </c>
+      <c r="L76" t="s">
+        <v>24</v>
+      </c>
+      <c r="M76" t="s">
+        <v>207</v>
+      </c>
+      <c r="N76" t="s">
+        <v>9</v>
+      </c>
+      <c r="O76" t="s">
+        <v>206</v>
+      </c>
+      <c r="P76" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q76" t="s">
+        <v>9</v>
+      </c>
+      <c r="R76" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="77" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C77" t="s">
+        <v>29</v>
+      </c>
+      <c r="D77">
+        <v>0.93500000000000005</v>
+      </c>
+      <c r="E77" t="s">
+        <v>9</v>
+      </c>
+      <c r="F77">
+        <v>58.771999999999998</v>
+      </c>
+      <c r="G77" t="s">
+        <v>9</v>
+      </c>
+      <c r="H77" t="s">
+        <v>9</v>
+      </c>
+      <c r="I77" t="s">
+        <v>9</v>
+      </c>
+      <c r="L77" t="s">
+        <v>29</v>
+      </c>
+      <c r="M77">
+        <v>1.4490000000000001</v>
+      </c>
+      <c r="N77" t="s">
+        <v>9</v>
+      </c>
+      <c r="O77">
+        <v>97.688000000000002</v>
+      </c>
+      <c r="P77" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q77" t="s">
+        <v>9</v>
+      </c>
+      <c r="R77">
+        <v>3.1179999999999999</v>
+      </c>
+    </row>
+    <row r="78" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B78" t="s">
+        <v>232</v>
+      </c>
+      <c r="C78" t="s">
+        <v>24</v>
+      </c>
+      <c r="D78" t="s">
+        <v>233</v>
+      </c>
+      <c r="E78" t="s">
+        <v>9</v>
+      </c>
+      <c r="F78" t="s">
+        <v>9</v>
+      </c>
+      <c r="G78" t="s">
+        <v>9</v>
+      </c>
+      <c r="H78" t="s">
+        <v>9</v>
+      </c>
+      <c r="I78" t="s">
+        <v>9</v>
+      </c>
+      <c r="K78" t="s">
+        <v>254</v>
+      </c>
+      <c r="L78" t="s">
+        <v>24</v>
+      </c>
+      <c r="M78" t="s">
+        <v>255</v>
+      </c>
+      <c r="N78" t="s">
+        <v>256</v>
+      </c>
+      <c r="O78" t="s">
+        <v>257</v>
+      </c>
+      <c r="P78" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q78" t="s">
+        <v>9</v>
+      </c>
+      <c r="R78" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="79" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C79" t="s">
+        <v>29</v>
+      </c>
+      <c r="D79">
+        <v>1.0509999999999999</v>
+      </c>
+      <c r="E79" t="s">
+        <v>9</v>
+      </c>
+      <c r="F79" t="s">
+        <v>9</v>
+      </c>
+      <c r="G79" t="s">
+        <v>9</v>
+      </c>
+      <c r="H79" t="s">
+        <v>9</v>
+      </c>
+      <c r="I79" t="s">
+        <v>9</v>
+      </c>
+      <c r="L79" t="s">
+        <v>29</v>
+      </c>
+      <c r="M79">
+        <v>1.63</v>
+      </c>
+      <c r="N79">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="O79">
+        <v>4.0460000000000003</v>
+      </c>
+      <c r="P79" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q79" t="s">
+        <v>9</v>
+      </c>
+      <c r="R79" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="80" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B80" t="s">
+        <v>178</v>
+      </c>
+      <c r="C80" t="s">
+        <v>24</v>
+      </c>
+      <c r="D80" t="s">
+        <v>234</v>
+      </c>
+      <c r="E80" t="s">
+        <v>9</v>
+      </c>
+      <c r="F80" t="s">
+        <v>235</v>
+      </c>
+      <c r="G80" t="s">
+        <v>9</v>
+      </c>
+      <c r="H80" t="s">
+        <v>9</v>
+      </c>
+      <c r="I80" t="s">
+        <v>236</v>
+      </c>
+      <c r="K80" t="s">
+        <v>258</v>
+      </c>
+      <c r="L80" t="s">
+        <v>24</v>
+      </c>
+      <c r="M80" t="s">
+        <v>259</v>
+      </c>
+      <c r="N80" t="s">
+        <v>9</v>
+      </c>
+      <c r="O80" t="s">
+        <v>260</v>
+      </c>
+      <c r="P80" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q80" t="s">
+        <v>9</v>
+      </c>
+      <c r="R80" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="81" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C81" t="s">
+        <v>29</v>
+      </c>
+      <c r="D81">
+        <v>1.1679999999999999</v>
+      </c>
+      <c r="E81" t="s">
+        <v>9</v>
+      </c>
+      <c r="F81">
+        <v>25.231999999999999</v>
+      </c>
+      <c r="G81" t="s">
+        <v>9</v>
+      </c>
+      <c r="H81" t="s">
+        <v>9</v>
+      </c>
+      <c r="I81">
+        <v>22.452999999999999</v>
+      </c>
+      <c r="L81" t="s">
+        <v>29</v>
+      </c>
+      <c r="M81">
+        <v>1.8120000000000001</v>
+      </c>
+      <c r="N81" t="s">
+        <v>9</v>
+      </c>
+      <c r="O81">
+        <v>4.2389999999999999</v>
+      </c>
+      <c r="P81" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q81" t="s">
+        <v>9</v>
+      </c>
+      <c r="R81" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="83" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B83" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="84" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B84" t="s">
+        <v>0</v>
+      </c>
+      <c r="C84" t="s">
+        <v>1</v>
+      </c>
+      <c r="D84" t="s">
+        <v>6</v>
+      </c>
+      <c r="E84" t="s">
+        <v>3</v>
+      </c>
+      <c r="F84" t="s">
+        <v>4</v>
+      </c>
+      <c r="G84" t="s">
+        <v>5</v>
+      </c>
+      <c r="H84" t="s">
+        <v>7</v>
+      </c>
+      <c r="I84" t="s">
+        <v>2</v>
+      </c>
+      <c r="K84" t="s">
+        <v>0</v>
+      </c>
+      <c r="L84" t="s">
+        <v>1</v>
+      </c>
+      <c r="M84" t="s">
+        <v>6</v>
+      </c>
+      <c r="N84" t="s">
+        <v>3</v>
+      </c>
+      <c r="O84" t="s">
+        <v>4</v>
+      </c>
+      <c r="P84" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q84" t="s">
+        <v>7</v>
+      </c>
+      <c r="R84" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B85" t="s">
+        <v>13</v>
+      </c>
+      <c r="C85" t="s">
+        <v>24</v>
+      </c>
+      <c r="D85" t="s">
+        <v>46</v>
+      </c>
+      <c r="E85" t="s">
+        <v>44</v>
+      </c>
+      <c r="F85" t="s">
+        <v>9</v>
+      </c>
+      <c r="G85" t="s">
+        <v>45</v>
+      </c>
+      <c r="H85" t="s">
+        <v>9</v>
+      </c>
+      <c r="I85" t="s">
+        <v>43</v>
+      </c>
+      <c r="K85" t="s">
+        <v>295</v>
+      </c>
+      <c r="L85" t="s">
+        <v>24</v>
+      </c>
+      <c r="M85" t="s">
+        <v>296</v>
+      </c>
+      <c r="N85" t="s">
+        <v>297</v>
+      </c>
+      <c r="O85" t="s">
+        <v>298</v>
+      </c>
+      <c r="P85" t="s">
+        <v>299</v>
+      </c>
+      <c r="Q85" t="s">
+        <v>9</v>
+      </c>
+      <c r="R85" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="86" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C86" t="s">
+        <v>29</v>
+      </c>
+      <c r="D86">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="E86">
+        <v>53.295999999999999</v>
+      </c>
+      <c r="F86" t="s">
+        <v>9</v>
+      </c>
+      <c r="G86">
+        <v>5.9580000000000002</v>
+      </c>
+      <c r="H86" t="s">
+        <v>9</v>
+      </c>
+      <c r="I86">
+        <v>0.45100000000000001</v>
+      </c>
+      <c r="L86" t="s">
+        <v>29</v>
+      </c>
+      <c r="M86">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="N86">
+        <v>83.37</v>
+      </c>
+      <c r="O86">
+        <v>44.893999999999998</v>
+      </c>
+      <c r="P86">
+        <v>5.0720000000000001</v>
+      </c>
+      <c r="Q86" t="s">
+        <v>9</v>
+      </c>
+      <c r="R86">
+        <v>8.6859999999999999</v>
+      </c>
+    </row>
+    <row r="87" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B87" t="s">
+        <v>263</v>
+      </c>
+      <c r="C87" t="s">
+        <v>24</v>
+      </c>
+      <c r="D87" t="s">
+        <v>264</v>
+      </c>
+      <c r="E87" t="s">
+        <v>265</v>
+      </c>
+      <c r="F87" t="s">
+        <v>266</v>
+      </c>
+      <c r="G87" t="s">
+        <v>267</v>
+      </c>
+      <c r="H87" t="s">
+        <v>268</v>
+      </c>
+      <c r="I87" t="s">
+        <v>269</v>
+      </c>
+      <c r="K87" t="s">
+        <v>301</v>
+      </c>
+      <c r="L87" t="s">
+        <v>24</v>
+      </c>
+      <c r="M87" t="s">
+        <v>302</v>
+      </c>
+      <c r="N87" t="s">
+        <v>303</v>
+      </c>
+      <c r="O87" t="s">
+        <v>304</v>
+      </c>
+      <c r="P87" t="s">
+        <v>305</v>
+      </c>
+      <c r="Q87" t="s">
+        <v>9</v>
+      </c>
+      <c r="R87" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="88" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C88" t="s">
+        <v>29</v>
+      </c>
+      <c r="D88">
+        <v>0.189</v>
+      </c>
+      <c r="E88">
+        <v>84.974999999999994</v>
+      </c>
+      <c r="F88">
+        <v>91.754000000000005</v>
+      </c>
+      <c r="G88">
+        <v>12.15</v>
+      </c>
+      <c r="H88">
+        <v>97.679000000000002</v>
+      </c>
+      <c r="I88">
+        <v>8.6560000000000006</v>
+      </c>
+      <c r="L88" t="s">
+        <v>29</v>
+      </c>
+      <c r="M88">
+        <v>0.32400000000000001</v>
+      </c>
+      <c r="N88">
+        <v>65.853999999999999</v>
+      </c>
+      <c r="O88">
+        <v>25.626000000000001</v>
+      </c>
+      <c r="P88">
+        <v>22.100999999999999</v>
+      </c>
+      <c r="Q88" t="s">
+        <v>9</v>
+      </c>
+      <c r="R88">
+        <v>21.158000000000001</v>
+      </c>
+    </row>
+    <row r="89" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B89" t="s">
+        <v>270</v>
+      </c>
+      <c r="C89" t="s">
+        <v>24</v>
+      </c>
+      <c r="D89" t="s">
+        <v>271</v>
+      </c>
+      <c r="E89" t="s">
+        <v>272</v>
+      </c>
+      <c r="F89" t="s">
+        <v>9</v>
+      </c>
+      <c r="G89" t="s">
+        <v>273</v>
+      </c>
+      <c r="H89" t="s">
+        <v>9</v>
+      </c>
+      <c r="I89" t="s">
+        <v>274</v>
+      </c>
+      <c r="K89" t="s">
+        <v>307</v>
+      </c>
+      <c r="L89" t="s">
+        <v>24</v>
+      </c>
+      <c r="M89" t="s">
+        <v>308</v>
+      </c>
+      <c r="N89" t="s">
+        <v>9</v>
+      </c>
+      <c r="O89" t="s">
+        <v>9</v>
+      </c>
+      <c r="P89" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q89" t="s">
+        <v>9</v>
+      </c>
+      <c r="R89" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="90" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C90" t="s">
+        <v>29</v>
+      </c>
+      <c r="D90">
+        <v>0.28399999999999997</v>
+      </c>
+      <c r="E90">
+        <v>42.097999999999999</v>
+      </c>
+      <c r="F90" t="s">
+        <v>9</v>
+      </c>
+      <c r="G90">
+        <v>24.416</v>
+      </c>
+      <c r="H90" t="s">
+        <v>9</v>
+      </c>
+      <c r="I90">
+        <v>15.148999999999999</v>
+      </c>
+      <c r="L90" t="s">
+        <v>29</v>
+      </c>
+      <c r="M90">
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="N90" t="s">
+        <v>9</v>
+      </c>
+      <c r="O90" t="s">
+        <v>9</v>
+      </c>
+      <c r="P90" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q90" t="s">
+        <v>9</v>
+      </c>
+      <c r="R90" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="91" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B91" t="s">
+        <v>275</v>
+      </c>
+      <c r="C91" t="s">
+        <v>24</v>
+      </c>
+      <c r="D91" t="s">
+        <v>276</v>
+      </c>
+      <c r="E91" t="s">
+        <v>9</v>
+      </c>
+      <c r="F91" t="s">
+        <v>277</v>
+      </c>
+      <c r="G91" t="s">
+        <v>9</v>
+      </c>
+      <c r="H91" t="s">
+        <v>9</v>
+      </c>
+      <c r="I91" t="s">
+        <v>278</v>
+      </c>
+      <c r="K91" t="s">
+        <v>309</v>
+      </c>
+      <c r="L91" t="s">
+        <v>24</v>
+      </c>
+      <c r="M91" t="s">
+        <v>310</v>
+      </c>
+      <c r="N91" t="s">
+        <v>9</v>
+      </c>
+      <c r="O91" t="s">
+        <v>311</v>
+      </c>
+      <c r="P91" t="s">
+        <v>312</v>
+      </c>
+      <c r="Q91" t="s">
+        <v>9</v>
+      </c>
+      <c r="R91" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="92" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C92" t="s">
+        <v>29</v>
+      </c>
+      <c r="D92">
+        <v>0.379</v>
+      </c>
+      <c r="E92" t="s">
+        <v>9</v>
+      </c>
+      <c r="F92">
+        <v>54.991</v>
+      </c>
+      <c r="G92" t="s">
+        <v>9</v>
+      </c>
+      <c r="H92" t="s">
+        <v>9</v>
+      </c>
+      <c r="I92">
+        <v>40.667000000000002</v>
+      </c>
+      <c r="L92" t="s">
+        <v>29</v>
+      </c>
+      <c r="M92">
+        <v>0.64700000000000002</v>
+      </c>
+      <c r="N92" t="s">
+        <v>9</v>
+      </c>
+      <c r="O92">
+        <v>79.960999999999999</v>
+      </c>
+      <c r="P92">
+        <v>88.948999999999998</v>
+      </c>
+      <c r="Q92" t="s">
+        <v>9</v>
+      </c>
+      <c r="R92">
+        <v>12.695</v>
+      </c>
+    </row>
+    <row r="93" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B93" t="s">
+        <v>279</v>
+      </c>
+      <c r="C93" t="s">
+        <v>24</v>
+      </c>
+      <c r="D93" t="s">
+        <v>276</v>
+      </c>
+      <c r="E93" t="s">
+        <v>9</v>
+      </c>
+      <c r="F93" t="s">
+        <v>9</v>
+      </c>
+      <c r="G93" t="s">
+        <v>9</v>
+      </c>
+      <c r="H93" t="s">
+        <v>9</v>
+      </c>
+      <c r="I93" t="s">
+        <v>9</v>
+      </c>
+      <c r="K93" t="s">
+        <v>314</v>
+      </c>
+      <c r="L93" t="s">
+        <v>24</v>
+      </c>
+      <c r="M93" t="s">
+        <v>315</v>
+      </c>
+      <c r="N93" t="s">
+        <v>9</v>
+      </c>
+      <c r="O93" t="s">
+        <v>316</v>
+      </c>
+      <c r="P93" t="s">
+        <v>317</v>
+      </c>
+      <c r="Q93" t="s">
+        <v>9</v>
+      </c>
+      <c r="R93" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="94" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C94" t="s">
+        <v>29</v>
+      </c>
+      <c r="D94">
+        <v>0.47299999999999998</v>
+      </c>
+      <c r="E94" t="s">
+        <v>9</v>
+      </c>
+      <c r="F94" t="s">
+        <v>9</v>
+      </c>
+      <c r="G94" t="s">
+        <v>9</v>
+      </c>
+      <c r="H94" t="s">
+        <v>9</v>
+      </c>
+      <c r="I94" t="s">
+        <v>9</v>
+      </c>
+      <c r="L94" t="s">
+        <v>29</v>
+      </c>
+      <c r="M94">
+        <v>0.80900000000000005</v>
+      </c>
+      <c r="N94" t="s">
+        <v>9</v>
+      </c>
+      <c r="O94">
+        <v>22.158000000000001</v>
+      </c>
+      <c r="P94">
+        <v>28.623000000000001</v>
+      </c>
+      <c r="Q94" t="s">
+        <v>9</v>
+      </c>
+      <c r="R94">
+        <v>33.408000000000001</v>
+      </c>
+    </row>
+    <row r="95" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B95" t="s">
+        <v>280</v>
+      </c>
+      <c r="C95" t="s">
+        <v>24</v>
+      </c>
+      <c r="D95" t="s">
+        <v>281</v>
+      </c>
+      <c r="E95" t="s">
+        <v>282</v>
+      </c>
+      <c r="F95" t="s">
+        <v>283</v>
+      </c>
+      <c r="G95" t="s">
+        <v>284</v>
+      </c>
+      <c r="H95" t="s">
+        <v>9</v>
+      </c>
+      <c r="I95" t="s">
+        <v>285</v>
+      </c>
+      <c r="K95" t="s">
+        <v>261</v>
+      </c>
+      <c r="L95" t="s">
+        <v>24</v>
+      </c>
+      <c r="M95" t="s">
+        <v>319</v>
+      </c>
+      <c r="N95" t="s">
+        <v>320</v>
+      </c>
+      <c r="O95" t="s">
+        <v>321</v>
+      </c>
+      <c r="P95" t="s">
+        <v>322</v>
+      </c>
+      <c r="Q95" t="s">
+        <v>9</v>
+      </c>
+      <c r="R95" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="96" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C96" t="s">
+        <v>29</v>
+      </c>
+      <c r="D96">
+        <v>0.56799999999999995</v>
+      </c>
+      <c r="E96">
+        <v>49.326999999999998</v>
+      </c>
+      <c r="F96">
+        <v>40.484000000000002</v>
+      </c>
+      <c r="G96">
+        <v>71.846000000000004</v>
+      </c>
+      <c r="H96" t="s">
+        <v>9</v>
+      </c>
+      <c r="I96">
+        <v>65.463999999999999</v>
+      </c>
+      <c r="L96" t="s">
+        <v>29</v>
+      </c>
+      <c r="M96">
+        <v>0.97099999999999997</v>
+      </c>
+      <c r="N96">
+        <v>25.942</v>
+      </c>
+      <c r="O96">
+        <v>9.4410000000000007</v>
+      </c>
+      <c r="P96">
+        <v>9.42</v>
+      </c>
+      <c r="Q96" t="s">
+        <v>9</v>
+      </c>
+      <c r="R96">
+        <v>5.5679999999999996</v>
+      </c>
+    </row>
+    <row r="97" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B97" t="s">
+        <v>286</v>
+      </c>
+      <c r="C97" t="s">
+        <v>24</v>
+      </c>
+      <c r="D97" t="s">
+        <v>281</v>
+      </c>
+      <c r="E97" t="s">
+        <v>9</v>
+      </c>
+      <c r="F97" t="s">
+        <v>9</v>
+      </c>
+      <c r="G97" t="s">
+        <v>9</v>
+      </c>
+      <c r="H97" t="s">
+        <v>9</v>
+      </c>
+      <c r="I97" t="s">
+        <v>9</v>
+      </c>
+      <c r="K97" t="s">
+        <v>324</v>
+      </c>
+      <c r="L97" t="s">
+        <v>24</v>
+      </c>
+      <c r="M97" t="s">
+        <v>325</v>
+      </c>
+      <c r="N97" t="s">
+        <v>9</v>
+      </c>
+      <c r="O97" t="s">
+        <v>9</v>
+      </c>
+      <c r="P97" t="s">
+        <v>326</v>
+      </c>
+      <c r="Q97" t="s">
+        <v>9</v>
+      </c>
+      <c r="R97" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="98" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C98" t="s">
+        <v>29</v>
+      </c>
+      <c r="D98">
+        <v>0.66300000000000003</v>
+      </c>
+      <c r="E98" t="s">
+        <v>9</v>
+      </c>
+      <c r="F98" t="s">
+        <v>9</v>
+      </c>
+      <c r="G98" t="s">
+        <v>9</v>
+      </c>
+      <c r="H98" t="s">
+        <v>9</v>
+      </c>
+      <c r="I98" t="s">
+        <v>9</v>
+      </c>
+      <c r="L98" t="s">
+        <v>29</v>
+      </c>
+      <c r="M98">
+        <v>1.133</v>
+      </c>
+      <c r="N98" t="s">
+        <v>9</v>
+      </c>
+      <c r="O98" t="s">
+        <v>9</v>
+      </c>
+      <c r="P98">
+        <v>5.6159999999999997</v>
+      </c>
+      <c r="Q98" t="s">
+        <v>9</v>
+      </c>
+      <c r="R98">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="99" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B99" t="s">
+        <v>287</v>
+      </c>
+      <c r="C99" t="s">
+        <v>24</v>
+      </c>
+      <c r="D99" t="s">
+        <v>281</v>
+      </c>
+      <c r="E99" t="s">
+        <v>9</v>
+      </c>
+      <c r="F99" t="s">
+        <v>9</v>
+      </c>
+      <c r="G99" t="s">
+        <v>9</v>
+      </c>
+      <c r="H99" t="s">
+        <v>9</v>
+      </c>
+      <c r="I99" t="s">
+        <v>9</v>
+      </c>
+      <c r="K99" t="s">
+        <v>328</v>
+      </c>
+      <c r="L99" t="s">
+        <v>24</v>
+      </c>
+      <c r="M99" t="s">
+        <v>329</v>
+      </c>
+      <c r="N99" t="s">
+        <v>330</v>
+      </c>
+      <c r="O99" t="s">
+        <v>331</v>
+      </c>
+      <c r="P99" t="s">
+        <v>332</v>
+      </c>
+      <c r="Q99" t="s">
+        <v>9</v>
+      </c>
+      <c r="R99" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="100" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C100" t="s">
+        <v>29</v>
+      </c>
+      <c r="D100">
+        <v>0.75800000000000001</v>
+      </c>
+      <c r="E100" t="s">
+        <v>9</v>
+      </c>
+      <c r="F100" t="s">
+        <v>9</v>
+      </c>
+      <c r="G100" t="s">
+        <v>9</v>
+      </c>
+      <c r="H100" t="s">
+        <v>9</v>
+      </c>
+      <c r="I100" t="s">
+        <v>9</v>
+      </c>
+      <c r="L100" t="s">
+        <v>29</v>
+      </c>
+      <c r="M100">
+        <v>1.294</v>
+      </c>
+      <c r="N100">
+        <v>23.725000000000001</v>
+      </c>
+      <c r="O100">
+        <v>12.138999999999999</v>
+      </c>
+      <c r="P100">
+        <v>16.123000000000001</v>
+      </c>
+      <c r="Q100" t="s">
+        <v>9</v>
+      </c>
+      <c r="R100">
+        <v>10.468</v>
+      </c>
+    </row>
+    <row r="101" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B101" t="s">
+        <v>288</v>
+      </c>
+      <c r="C101" t="s">
+        <v>24</v>
+      </c>
+      <c r="D101" t="s">
+        <v>281</v>
+      </c>
+      <c r="E101" t="s">
+        <v>289</v>
+      </c>
+      <c r="F101" t="s">
+        <v>290</v>
+      </c>
+      <c r="G101" t="s">
+        <v>291</v>
+      </c>
+      <c r="H101" t="s">
+        <v>9</v>
+      </c>
+      <c r="I101" t="s">
+        <v>292</v>
+      </c>
+      <c r="K101" t="s">
+        <v>262</v>
+      </c>
+      <c r="L101" t="s">
+        <v>24</v>
+      </c>
+      <c r="M101" t="s">
+        <v>334</v>
+      </c>
+      <c r="N101" t="s">
+        <v>335</v>
+      </c>
+      <c r="O101" t="s">
+        <v>336</v>
+      </c>
+      <c r="P101" t="s">
+        <v>337</v>
+      </c>
+      <c r="Q101" t="s">
+        <v>9</v>
+      </c>
+      <c r="R101" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="102" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C102" t="s">
+        <v>29</v>
+      </c>
+      <c r="D102">
+        <v>0.85199999999999998</v>
+      </c>
+      <c r="E102">
+        <v>51.381999999999998</v>
+      </c>
+      <c r="F102">
+        <v>40.793999999999997</v>
+      </c>
+      <c r="G102">
+        <v>35.981000000000002</v>
+      </c>
+      <c r="H102" t="s">
+        <v>9</v>
+      </c>
+      <c r="I102">
+        <v>39.405000000000001</v>
+      </c>
+      <c r="L102" t="s">
+        <v>29</v>
+      </c>
+      <c r="M102">
+        <v>1.456</v>
+      </c>
+      <c r="N102">
+        <v>15.743</v>
+      </c>
+      <c r="O102">
+        <v>11.946</v>
+      </c>
+      <c r="P102">
+        <v>11.593999999999999</v>
+      </c>
+      <c r="Q102" t="s">
+        <v>9</v>
+      </c>
+      <c r="R102">
+        <v>6.9039999999999999</v>
+      </c>
+    </row>
+    <row r="103" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B103" t="s">
+        <v>293</v>
+      </c>
+      <c r="C103" t="s">
+        <v>24</v>
+      </c>
+      <c r="D103" t="s">
+        <v>294</v>
+      </c>
+      <c r="E103" t="s">
+        <v>9</v>
+      </c>
+      <c r="F103" t="s">
+        <v>9</v>
+      </c>
+      <c r="G103" t="s">
+        <v>9</v>
+      </c>
+      <c r="H103" t="s">
+        <v>9</v>
+      </c>
+      <c r="I103" t="s">
+        <v>9</v>
+      </c>
+      <c r="K103" t="s">
+        <v>339</v>
+      </c>
+      <c r="L103" t="s">
+        <v>24</v>
+      </c>
+      <c r="M103" t="s">
+        <v>340</v>
+      </c>
+      <c r="N103" t="s">
+        <v>9</v>
+      </c>
+      <c r="O103" t="s">
+        <v>9</v>
+      </c>
+      <c r="P103" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q103" t="s">
+        <v>9</v>
+      </c>
+      <c r="R103" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="104" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C104" t="s">
+        <v>29</v>
+      </c>
+      <c r="D104">
+        <v>0.94699999999999995</v>
+      </c>
+      <c r="E104" t="s">
+        <v>9</v>
+      </c>
+      <c r="F104" t="s">
+        <v>9</v>
+      </c>
+      <c r="G104" t="s">
+        <v>9</v>
+      </c>
+      <c r="H104" t="s">
+        <v>9</v>
+      </c>
+      <c r="I104" t="s">
+        <v>9</v>
+      </c>
+      <c r="L104" t="s">
+        <v>29</v>
+      </c>
+      <c r="M104">
+        <v>1.6180000000000001</v>
+      </c>
+      <c r="N104" t="s">
+        <v>9</v>
+      </c>
+      <c r="O104" t="s">
+        <v>9</v>
+      </c>
+      <c r="P104" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q104" t="s">
+        <v>9</v>
+      </c>
+      <c r="R104" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update rank tables; export go_only
</commit_message>
<xml_diff>
--- a/results/legacy/rank_tables_comparison.xlsx
+++ b/results/legacy/rank_tables_comparison.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rsajulga/Projects/umn/galaxyp/functional-tools-survey/functional-analysis-benchmarking/results/legacy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{408F095F-8CD5-984A-8578-A4AE7E07C9E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CC8FFEC-154A-374B-A4B4-BB7377C597F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-560" yWindow="460" windowWidth="32780" windowHeight="18320" activeTab="1" xr2:uid="{0B4038EE-9BFE-1546-B252-9856E1BA96F5}"/>
+    <workbookView xWindow="6100" yWindow="1620" windowWidth="26560" windowHeight="20360" activeTab="2" xr2:uid="{0B4038EE-9BFE-1546-B252-9856E1BA96F5}"/>
   </bookViews>
   <sheets>
     <sheet name="040720" sheetId="1" r:id="rId1"/>
     <sheet name="041420" sheetId="2" r:id="rId2"/>
+    <sheet name="042020 (2)" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2288" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2915" uniqueCount="403">
   <si>
     <t>GO Term</t>
   </si>
@@ -1216,6 +1217,33 @@
   </si>
   <si>
     <t>0.19 (6.64 / 5.7)</t>
+  </si>
+  <si>
+    <t>0.07 (-9.76 / -9.37)</t>
+  </si>
+  <si>
+    <t>-0.5 (4.46 / 6.71)</t>
+  </si>
+  <si>
+    <t>0.3 (9.19 / 7.29)</t>
+  </si>
+  <si>
+    <t>-0.54 (-7 / -9.69)</t>
+  </si>
+  <si>
+    <t>0.33 (8.74 / 6.75)</t>
+  </si>
+  <si>
+    <t>0.16 (6.67 / 5.88)</t>
+  </si>
+  <si>
+    <t>0.16 (-5.5 / -5.03)</t>
+  </si>
+  <si>
+    <t>0.24 (10.71 / 8.93)</t>
+  </si>
+  <si>
+    <t>0.47 (0.04 / 0.03)</t>
   </si>
 </sst>
 </file>
@@ -6074,7 +6102,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B929CB3-0F32-FC4E-9739-69EA2331ACF1}">
   <dimension ref="B1:R104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
@@ -10555,4 +10583,2507 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84589D99-C837-6449-8CA7-00B2780B4E93}">
+  <dimension ref="B1:R83"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="P29" sqref="P29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="24.33203125" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" customWidth="1"/>
+    <col min="11" max="11" width="25.6640625" customWidth="1"/>
+    <col min="12" max="12" width="18.83203125" customWidth="1"/>
+    <col min="13" max="13" width="20.5" customWidth="1"/>
+    <col min="14" max="14" width="18.33203125" customWidth="1"/>
+    <col min="15" max="15" width="25.1640625" customWidth="1"/>
+    <col min="16" max="16" width="12.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B1" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="3" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B3" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" t="s">
+        <v>2</v>
+      </c>
+      <c r="K4" t="s">
+        <v>0</v>
+      </c>
+      <c r="L4" t="s">
+        <v>1</v>
+      </c>
+      <c r="M4" t="s">
+        <v>3</v>
+      </c>
+      <c r="N4" t="s">
+        <v>4</v>
+      </c>
+      <c r="O4" t="s">
+        <v>5</v>
+      </c>
+      <c r="P4" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>7</v>
+      </c>
+      <c r="R4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" t="s">
+        <v>86</v>
+      </c>
+      <c r="H5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K5" t="s">
+        <v>131</v>
+      </c>
+      <c r="L5" t="s">
+        <v>24</v>
+      </c>
+      <c r="M5" t="s">
+        <v>132</v>
+      </c>
+      <c r="N5" t="s">
+        <v>133</v>
+      </c>
+      <c r="O5" t="s">
+        <v>9</v>
+      </c>
+      <c r="P5" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>9</v>
+      </c>
+      <c r="R5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="E6">
+        <v>13.887</v>
+      </c>
+      <c r="F6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6">
+        <v>72.555000000000007</v>
+      </c>
+      <c r="H6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" t="s">
+        <v>9</v>
+      </c>
+      <c r="L6" t="s">
+        <v>29</v>
+      </c>
+      <c r="M6">
+        <v>0.31</v>
+      </c>
+      <c r="N6">
+        <v>38.965000000000003</v>
+      </c>
+      <c r="O6" t="s">
+        <v>9</v>
+      </c>
+      <c r="P6" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>9</v>
+      </c>
+      <c r="R6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>88</v>
+      </c>
+      <c r="E7" t="s">
+        <v>89</v>
+      </c>
+      <c r="F7" t="s">
+        <v>90</v>
+      </c>
+      <c r="G7" t="s">
+        <v>91</v>
+      </c>
+      <c r="H7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7" t="s">
+        <v>92</v>
+      </c>
+      <c r="K7" t="s">
+        <v>143</v>
+      </c>
+      <c r="L7" t="s">
+        <v>24</v>
+      </c>
+      <c r="M7" t="s">
+        <v>144</v>
+      </c>
+      <c r="N7" t="s">
+        <v>145</v>
+      </c>
+      <c r="O7" t="s">
+        <v>9</v>
+      </c>
+      <c r="P7" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>394</v>
+      </c>
+      <c r="R7" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="E8">
+        <v>33.043999999999997</v>
+      </c>
+      <c r="F8">
+        <v>37.85</v>
+      </c>
+      <c r="G8">
+        <v>43.375</v>
+      </c>
+      <c r="H8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I8">
+        <v>33.994999999999997</v>
+      </c>
+      <c r="L8" t="s">
+        <v>29</v>
+      </c>
+      <c r="M8">
+        <v>0.61899999999999999</v>
+      </c>
+      <c r="N8">
+        <v>34.06</v>
+      </c>
+      <c r="O8" t="s">
+        <v>9</v>
+      </c>
+      <c r="P8" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q8">
+        <v>18.681000000000001</v>
+      </c>
+      <c r="R8">
+        <v>97.522999999999996</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" t="s">
+        <v>94</v>
+      </c>
+      <c r="E9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9" t="s">
+        <v>9</v>
+      </c>
+      <c r="K9" t="s">
+        <v>148</v>
+      </c>
+      <c r="L9" t="s">
+        <v>24</v>
+      </c>
+      <c r="M9" t="s">
+        <v>149</v>
+      </c>
+      <c r="N9" t="s">
+        <v>150</v>
+      </c>
+      <c r="O9" t="s">
+        <v>151</v>
+      </c>
+      <c r="P9" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>9</v>
+      </c>
+      <c r="R9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10">
+        <v>0.21299999999999999</v>
+      </c>
+      <c r="E10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" t="s">
+        <v>9</v>
+      </c>
+      <c r="I10" t="s">
+        <v>9</v>
+      </c>
+      <c r="L10" t="s">
+        <v>29</v>
+      </c>
+      <c r="M10">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="N10">
+        <v>15.259</v>
+      </c>
+      <c r="O10">
+        <v>11.417</v>
+      </c>
+      <c r="P10" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>9</v>
+      </c>
+      <c r="R10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>95</v>
+      </c>
+      <c r="C11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" t="s">
+        <v>94</v>
+      </c>
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" t="s">
+        <v>9</v>
+      </c>
+      <c r="I11" t="s">
+        <v>9</v>
+      </c>
+      <c r="K11" t="s">
+        <v>342</v>
+      </c>
+      <c r="L11" t="s">
+        <v>24</v>
+      </c>
+      <c r="M11" t="s">
+        <v>343</v>
+      </c>
+      <c r="N11" t="s">
+        <v>9</v>
+      </c>
+      <c r="O11" t="s">
+        <v>9</v>
+      </c>
+      <c r="P11" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>9</v>
+      </c>
+      <c r="R11" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12">
+        <v>0.28299999999999997</v>
+      </c>
+      <c r="E12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" t="s">
+        <v>9</v>
+      </c>
+      <c r="H12" t="s">
+        <v>9</v>
+      </c>
+      <c r="I12" t="s">
+        <v>9</v>
+      </c>
+      <c r="L12" t="s">
+        <v>29</v>
+      </c>
+      <c r="M12">
+        <v>1.238</v>
+      </c>
+      <c r="N12" t="s">
+        <v>9</v>
+      </c>
+      <c r="O12" t="s">
+        <v>9</v>
+      </c>
+      <c r="P12" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>9</v>
+      </c>
+      <c r="R12">
+        <v>42.104999999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>96</v>
+      </c>
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" t="s">
+        <v>94</v>
+      </c>
+      <c r="E13" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" t="s">
+        <v>97</v>
+      </c>
+      <c r="G13" t="s">
+        <v>9</v>
+      </c>
+      <c r="H13" t="s">
+        <v>9</v>
+      </c>
+      <c r="I13" t="s">
+        <v>9</v>
+      </c>
+      <c r="K13" t="s">
+        <v>103</v>
+      </c>
+      <c r="L13" t="s">
+        <v>24</v>
+      </c>
+      <c r="M13" t="s">
+        <v>345</v>
+      </c>
+      <c r="N13" t="s">
+        <v>346</v>
+      </c>
+      <c r="O13" t="s">
+        <v>9</v>
+      </c>
+      <c r="P13" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>9</v>
+      </c>
+      <c r="R13" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14">
+        <v>0.35399999999999998</v>
+      </c>
+      <c r="E14">
+        <v>29.076000000000001</v>
+      </c>
+      <c r="F14">
+        <v>74.533000000000001</v>
+      </c>
+      <c r="G14" t="s">
+        <v>9</v>
+      </c>
+      <c r="H14" t="s">
+        <v>9</v>
+      </c>
+      <c r="I14" t="s">
+        <v>9</v>
+      </c>
+      <c r="L14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M14">
+        <v>1.548</v>
+      </c>
+      <c r="N14">
+        <v>10.627000000000001</v>
+      </c>
+      <c r="O14" t="s">
+        <v>9</v>
+      </c>
+      <c r="P14" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>9</v>
+      </c>
+      <c r="R14">
+        <v>19.195</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>98</v>
+      </c>
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" t="s">
+        <v>99</v>
+      </c>
+      <c r="E15" t="s">
+        <v>100</v>
+      </c>
+      <c r="F15" t="s">
+        <v>101</v>
+      </c>
+      <c r="G15" t="s">
+        <v>9</v>
+      </c>
+      <c r="H15" t="s">
+        <v>9</v>
+      </c>
+      <c r="I15" t="s">
+        <v>102</v>
+      </c>
+      <c r="K15" t="s">
+        <v>349</v>
+      </c>
+      <c r="L15" t="s">
+        <v>24</v>
+      </c>
+      <c r="M15" t="s">
+        <v>350</v>
+      </c>
+      <c r="N15" t="s">
+        <v>9</v>
+      </c>
+      <c r="O15" t="s">
+        <v>9</v>
+      </c>
+      <c r="P15" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>9</v>
+      </c>
+      <c r="R15" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16">
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="E16">
+        <v>5.0839999999999996</v>
+      </c>
+      <c r="F16">
+        <v>12.967000000000001</v>
+      </c>
+      <c r="G16" t="s">
+        <v>9</v>
+      </c>
+      <c r="H16" t="s">
+        <v>9</v>
+      </c>
+      <c r="I16">
+        <v>3.1560000000000001</v>
+      </c>
+      <c r="L16" t="s">
+        <v>29</v>
+      </c>
+      <c r="M16">
+        <v>1.8580000000000001</v>
+      </c>
+      <c r="N16" t="s">
+        <v>9</v>
+      </c>
+      <c r="O16" t="s">
+        <v>9</v>
+      </c>
+      <c r="P16" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>9</v>
+      </c>
+      <c r="R16">
+        <v>42.414999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>103</v>
+      </c>
+      <c r="C17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" t="s">
+        <v>104</v>
+      </c>
+      <c r="E17" t="s">
+        <v>105</v>
+      </c>
+      <c r="F17" t="s">
+        <v>106</v>
+      </c>
+      <c r="G17" t="s">
+        <v>9</v>
+      </c>
+      <c r="H17" t="s">
+        <v>9</v>
+      </c>
+      <c r="I17" t="s">
+        <v>107</v>
+      </c>
+      <c r="K17" t="s">
+        <v>185</v>
+      </c>
+      <c r="L17" t="s">
+        <v>24</v>
+      </c>
+      <c r="M17" t="s">
+        <v>187</v>
+      </c>
+      <c r="N17" t="s">
+        <v>9</v>
+      </c>
+      <c r="O17" t="s">
+        <v>9</v>
+      </c>
+      <c r="P17" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>9</v>
+      </c>
+      <c r="R17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18">
+        <v>0.496</v>
+      </c>
+      <c r="E18">
+        <v>30.687999999999999</v>
+      </c>
+      <c r="F18">
+        <v>36.215000000000003</v>
+      </c>
+      <c r="G18" t="s">
+        <v>9</v>
+      </c>
+      <c r="H18" t="s">
+        <v>9</v>
+      </c>
+      <c r="I18">
+        <v>79.981999999999999</v>
+      </c>
+      <c r="L18" t="s">
+        <v>29</v>
+      </c>
+      <c r="M18">
+        <v>2.1669999999999998</v>
+      </c>
+      <c r="N18" t="s">
+        <v>9</v>
+      </c>
+      <c r="O18" t="s">
+        <v>9</v>
+      </c>
+      <c r="P18" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>9</v>
+      </c>
+      <c r="R18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>108</v>
+      </c>
+      <c r="C19" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" t="s">
+        <v>109</v>
+      </c>
+      <c r="E19" t="s">
+        <v>110</v>
+      </c>
+      <c r="F19" t="s">
+        <v>9</v>
+      </c>
+      <c r="G19" t="s">
+        <v>9</v>
+      </c>
+      <c r="H19" t="s">
+        <v>9</v>
+      </c>
+      <c r="I19" t="s">
+        <v>9</v>
+      </c>
+      <c r="K19" t="s">
+        <v>351</v>
+      </c>
+      <c r="L19" t="s">
+        <v>24</v>
+      </c>
+      <c r="M19" t="s">
+        <v>352</v>
+      </c>
+      <c r="N19" t="s">
+        <v>353</v>
+      </c>
+      <c r="O19" t="s">
+        <v>9</v>
+      </c>
+      <c r="P19" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>9</v>
+      </c>
+      <c r="R19" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="20" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20">
+        <v>0.56699999999999995</v>
+      </c>
+      <c r="E20">
+        <v>10.911</v>
+      </c>
+      <c r="F20" t="s">
+        <v>9</v>
+      </c>
+      <c r="G20" t="s">
+        <v>9</v>
+      </c>
+      <c r="H20" t="s">
+        <v>9</v>
+      </c>
+      <c r="I20" t="s">
+        <v>9</v>
+      </c>
+      <c r="L20" t="s">
+        <v>29</v>
+      </c>
+      <c r="M20">
+        <v>2.4769999999999999</v>
+      </c>
+      <c r="N20">
+        <v>17.710999999999999</v>
+      </c>
+      <c r="O20" t="s">
+        <v>9</v>
+      </c>
+      <c r="P20" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>9</v>
+      </c>
+      <c r="R20">
+        <v>20.433</v>
+      </c>
+    </row>
+    <row r="21" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>111</v>
+      </c>
+      <c r="C21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" t="s">
+        <v>112</v>
+      </c>
+      <c r="E21" t="s">
+        <v>113</v>
+      </c>
+      <c r="F21" t="s">
+        <v>114</v>
+      </c>
+      <c r="G21" t="s">
+        <v>9</v>
+      </c>
+      <c r="H21" t="s">
+        <v>9</v>
+      </c>
+      <c r="I21" t="s">
+        <v>115</v>
+      </c>
+      <c r="K21" t="s">
+        <v>356</v>
+      </c>
+      <c r="L21" t="s">
+        <v>24</v>
+      </c>
+      <c r="M21" t="s">
+        <v>357</v>
+      </c>
+      <c r="N21" t="s">
+        <v>358</v>
+      </c>
+      <c r="O21" t="s">
+        <v>9</v>
+      </c>
+      <c r="P21" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>9</v>
+      </c>
+      <c r="R21" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="22" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C22" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22">
+        <v>0.63800000000000001</v>
+      </c>
+      <c r="E22">
+        <v>41.970999999999997</v>
+      </c>
+      <c r="F22">
+        <v>74.882999999999996</v>
+      </c>
+      <c r="G22" t="s">
+        <v>9</v>
+      </c>
+      <c r="H22" t="s">
+        <v>9</v>
+      </c>
+      <c r="I22">
+        <v>78.179000000000002</v>
+      </c>
+      <c r="L22" t="s">
+        <v>29</v>
+      </c>
+      <c r="M22">
+        <v>2.786</v>
+      </c>
+      <c r="N22">
+        <v>21.526</v>
+      </c>
+      <c r="O22" t="s">
+        <v>9</v>
+      </c>
+      <c r="P22" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>9</v>
+      </c>
+      <c r="R22">
+        <v>24.149000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>116</v>
+      </c>
+      <c r="C23" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" t="s">
+        <v>117</v>
+      </c>
+      <c r="E23" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" t="s">
+        <v>9</v>
+      </c>
+      <c r="G23" t="s">
+        <v>9</v>
+      </c>
+      <c r="H23" t="s">
+        <v>9</v>
+      </c>
+      <c r="I23" t="s">
+        <v>9</v>
+      </c>
+      <c r="K23" t="s">
+        <v>361</v>
+      </c>
+      <c r="L23" t="s">
+        <v>24</v>
+      </c>
+      <c r="M23" t="s">
+        <v>343</v>
+      </c>
+      <c r="N23" t="s">
+        <v>9</v>
+      </c>
+      <c r="O23" t="s">
+        <v>9</v>
+      </c>
+      <c r="P23" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>9</v>
+      </c>
+      <c r="R23" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="24" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C24" t="s">
+        <v>29</v>
+      </c>
+      <c r="D24">
+        <v>0.70899999999999996</v>
+      </c>
+      <c r="E24" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" t="s">
+        <v>9</v>
+      </c>
+      <c r="G24" t="s">
+        <v>9</v>
+      </c>
+      <c r="H24" t="s">
+        <v>9</v>
+      </c>
+      <c r="I24" t="s">
+        <v>9</v>
+      </c>
+      <c r="L24" t="s">
+        <v>29</v>
+      </c>
+      <c r="M24">
+        <v>1.238</v>
+      </c>
+      <c r="N24" t="s">
+        <v>9</v>
+      </c>
+      <c r="O24" t="s">
+        <v>9</v>
+      </c>
+      <c r="P24" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>9</v>
+      </c>
+      <c r="R24">
+        <v>42.104999999999997</v>
+      </c>
+    </row>
+    <row r="26" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B26" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="27" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" t="s">
+        <v>1</v>
+      </c>
+      <c r="D27" t="s">
+        <v>2</v>
+      </c>
+      <c r="E27" t="s">
+        <v>3</v>
+      </c>
+      <c r="F27" t="s">
+        <v>4</v>
+      </c>
+      <c r="G27" t="s">
+        <v>5</v>
+      </c>
+      <c r="H27" t="s">
+        <v>6</v>
+      </c>
+      <c r="I27" t="s">
+        <v>7</v>
+      </c>
+      <c r="K27" t="s">
+        <v>0</v>
+      </c>
+      <c r="L27" t="s">
+        <v>1</v>
+      </c>
+      <c r="M27" t="s">
+        <v>2</v>
+      </c>
+      <c r="N27" t="s">
+        <v>3</v>
+      </c>
+      <c r="O27" t="s">
+        <v>4</v>
+      </c>
+      <c r="P27" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>6</v>
+      </c>
+      <c r="R27" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" t="s">
+        <v>24</v>
+      </c>
+      <c r="D28" t="s">
+        <v>25</v>
+      </c>
+      <c r="E28" t="s">
+        <v>26</v>
+      </c>
+      <c r="F28" t="s">
+        <v>27</v>
+      </c>
+      <c r="G28" t="s">
+        <v>28</v>
+      </c>
+      <c r="H28" t="s">
+        <v>9</v>
+      </c>
+      <c r="I28" t="s">
+        <v>9</v>
+      </c>
+      <c r="K28" t="s">
+        <v>175</v>
+      </c>
+      <c r="L28" t="s">
+        <v>24</v>
+      </c>
+      <c r="M28" t="s">
+        <v>176</v>
+      </c>
+      <c r="N28" t="s">
+        <v>9</v>
+      </c>
+      <c r="O28" t="s">
+        <v>177</v>
+      </c>
+      <c r="P28" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>9</v>
+      </c>
+      <c r="R28" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C29" t="s">
+        <v>29</v>
+      </c>
+      <c r="D29">
+        <v>0.09</v>
+      </c>
+      <c r="E29">
+        <v>67.328000000000003</v>
+      </c>
+      <c r="F29">
+        <v>0.434</v>
+      </c>
+      <c r="G29">
+        <v>2.57</v>
+      </c>
+      <c r="H29" t="s">
+        <v>9</v>
+      </c>
+      <c r="I29" t="s">
+        <v>9</v>
+      </c>
+      <c r="L29" t="s">
+        <v>29</v>
+      </c>
+      <c r="M29">
+        <v>0.31</v>
+      </c>
+      <c r="N29" t="s">
+        <v>9</v>
+      </c>
+      <c r="O29">
+        <v>11.444000000000001</v>
+      </c>
+      <c r="P29" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>9</v>
+      </c>
+      <c r="R29" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" t="s">
+        <v>24</v>
+      </c>
+      <c r="D30" t="s">
+        <v>30</v>
+      </c>
+      <c r="E30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" t="s">
+        <v>31</v>
+      </c>
+      <c r="G30" t="s">
+        <v>32</v>
+      </c>
+      <c r="H30" t="s">
+        <v>33</v>
+      </c>
+      <c r="I30" t="s">
+        <v>9</v>
+      </c>
+      <c r="K30" t="s">
+        <v>178</v>
+      </c>
+      <c r="L30" t="s">
+        <v>24</v>
+      </c>
+      <c r="M30" t="s">
+        <v>179</v>
+      </c>
+      <c r="N30" t="s">
+        <v>9</v>
+      </c>
+      <c r="O30" t="s">
+        <v>9</v>
+      </c>
+      <c r="P30" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>9</v>
+      </c>
+      <c r="R30" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C31" t="s">
+        <v>29</v>
+      </c>
+      <c r="D31">
+        <v>0.18</v>
+      </c>
+      <c r="E31" t="s">
+        <v>9</v>
+      </c>
+      <c r="F31">
+        <v>1.054</v>
+      </c>
+      <c r="G31">
+        <v>1.2849999999999999</v>
+      </c>
+      <c r="H31">
+        <v>29.18</v>
+      </c>
+      <c r="I31" t="s">
+        <v>9</v>
+      </c>
+      <c r="L31" t="s">
+        <v>29</v>
+      </c>
+      <c r="M31">
+        <v>0.61899999999999999</v>
+      </c>
+      <c r="N31" t="s">
+        <v>9</v>
+      </c>
+      <c r="O31" t="s">
+        <v>9</v>
+      </c>
+      <c r="P31" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>9</v>
+      </c>
+      <c r="R31" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" t="s">
+        <v>24</v>
+      </c>
+      <c r="D32" t="s">
+        <v>34</v>
+      </c>
+      <c r="E32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32" t="s">
+        <v>35</v>
+      </c>
+      <c r="G32" t="s">
+        <v>36</v>
+      </c>
+      <c r="H32" t="s">
+        <v>37</v>
+      </c>
+      <c r="I32" t="s">
+        <v>9</v>
+      </c>
+      <c r="K32" t="s">
+        <v>196</v>
+      </c>
+      <c r="L32" t="s">
+        <v>24</v>
+      </c>
+      <c r="M32" t="s">
+        <v>197</v>
+      </c>
+      <c r="N32" t="s">
+        <v>9</v>
+      </c>
+      <c r="O32" t="s">
+        <v>9</v>
+      </c>
+      <c r="P32" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>9</v>
+      </c>
+      <c r="R32" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C33" t="s">
+        <v>29</v>
+      </c>
+      <c r="D33">
+        <v>0.27100000000000002</v>
+      </c>
+      <c r="E33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F33">
+        <v>0.99199999999999999</v>
+      </c>
+      <c r="G33">
+        <v>2.9209999999999998</v>
+      </c>
+      <c r="H33">
+        <v>4.4160000000000004</v>
+      </c>
+      <c r="I33" t="s">
+        <v>9</v>
+      </c>
+      <c r="L33" t="s">
+        <v>29</v>
+      </c>
+      <c r="M33">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="N33" t="s">
+        <v>9</v>
+      </c>
+      <c r="O33" t="s">
+        <v>9</v>
+      </c>
+      <c r="P33">
+        <v>3.5430000000000001</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>9</v>
+      </c>
+      <c r="R33" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>12</v>
+      </c>
+      <c r="C34" t="s">
+        <v>24</v>
+      </c>
+      <c r="D34" t="s">
+        <v>38</v>
+      </c>
+      <c r="E34" t="s">
+        <v>39</v>
+      </c>
+      <c r="F34" t="s">
+        <v>40</v>
+      </c>
+      <c r="G34" t="s">
+        <v>41</v>
+      </c>
+      <c r="H34" t="s">
+        <v>42</v>
+      </c>
+      <c r="I34" t="s">
+        <v>9</v>
+      </c>
+      <c r="K34" t="s">
+        <v>199</v>
+      </c>
+      <c r="L34" t="s">
+        <v>24</v>
+      </c>
+      <c r="M34" t="s">
+        <v>197</v>
+      </c>
+      <c r="N34" t="s">
+        <v>9</v>
+      </c>
+      <c r="O34" t="s">
+        <v>9</v>
+      </c>
+      <c r="P34" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>9</v>
+      </c>
+      <c r="R34" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C35" t="s">
+        <v>29</v>
+      </c>
+      <c r="D35">
+        <v>0.36099999999999999</v>
+      </c>
+      <c r="E35">
+        <v>94.685000000000002</v>
+      </c>
+      <c r="F35">
+        <v>18.722999999999999</v>
+      </c>
+      <c r="G35">
+        <v>40.186999999999998</v>
+      </c>
+      <c r="H35">
+        <v>3.9430000000000001</v>
+      </c>
+      <c r="I35" t="s">
+        <v>9</v>
+      </c>
+      <c r="L35" t="s">
+        <v>29</v>
+      </c>
+      <c r="M35">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="N35" t="s">
+        <v>9</v>
+      </c>
+      <c r="O35" t="s">
+        <v>9</v>
+      </c>
+      <c r="P35">
+        <v>3.5430000000000001</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>9</v>
+      </c>
+      <c r="R35" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" t="s">
+        <v>24</v>
+      </c>
+      <c r="D36" t="s">
+        <v>43</v>
+      </c>
+      <c r="E36" t="s">
+        <v>44</v>
+      </c>
+      <c r="F36" t="s">
+        <v>9</v>
+      </c>
+      <c r="G36" t="s">
+        <v>45</v>
+      </c>
+      <c r="H36" t="s">
+        <v>46</v>
+      </c>
+      <c r="I36" t="s">
+        <v>9</v>
+      </c>
+      <c r="K36" t="s">
+        <v>362</v>
+      </c>
+      <c r="L36" t="s">
+        <v>24</v>
+      </c>
+      <c r="M36" t="s">
+        <v>363</v>
+      </c>
+      <c r="N36" t="s">
+        <v>9</v>
+      </c>
+      <c r="O36" t="s">
+        <v>9</v>
+      </c>
+      <c r="P36" t="s">
+        <v>364</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>9</v>
+      </c>
+      <c r="R36" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C37" t="s">
+        <v>29</v>
+      </c>
+      <c r="D37">
+        <v>0.45100000000000001</v>
+      </c>
+      <c r="E37">
+        <v>53.295999999999999</v>
+      </c>
+      <c r="F37" t="s">
+        <v>9</v>
+      </c>
+      <c r="G37">
+        <v>5.9580000000000002</v>
+      </c>
+      <c r="H37">
+        <v>0.158</v>
+      </c>
+      <c r="I37" t="s">
+        <v>9</v>
+      </c>
+      <c r="L37" t="s">
+        <v>29</v>
+      </c>
+      <c r="M37">
+        <v>1.548</v>
+      </c>
+      <c r="N37" t="s">
+        <v>9</v>
+      </c>
+      <c r="O37" t="s">
+        <v>9</v>
+      </c>
+      <c r="P37">
+        <v>5.1180000000000003</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>9</v>
+      </c>
+      <c r="R37" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" t="s">
+        <v>24</v>
+      </c>
+      <c r="D38" t="s">
+        <v>47</v>
+      </c>
+      <c r="E38" t="s">
+        <v>9</v>
+      </c>
+      <c r="F38" t="s">
+        <v>48</v>
+      </c>
+      <c r="G38" t="s">
+        <v>49</v>
+      </c>
+      <c r="H38" t="s">
+        <v>9</v>
+      </c>
+      <c r="I38" t="s">
+        <v>9</v>
+      </c>
+      <c r="K38" t="s">
+        <v>324</v>
+      </c>
+      <c r="L38" t="s">
+        <v>24</v>
+      </c>
+      <c r="M38" t="s">
+        <v>327</v>
+      </c>
+      <c r="N38" t="s">
+        <v>9</v>
+      </c>
+      <c r="O38" t="s">
+        <v>9</v>
+      </c>
+      <c r="P38" t="s">
+        <v>326</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>9</v>
+      </c>
+      <c r="R38" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C39" t="s">
+        <v>29</v>
+      </c>
+      <c r="D39">
+        <v>0.54100000000000004</v>
+      </c>
+      <c r="E39" t="s">
+        <v>9</v>
+      </c>
+      <c r="F39">
+        <v>2.17</v>
+      </c>
+      <c r="G39">
+        <v>2.6869999999999998</v>
+      </c>
+      <c r="H39" t="s">
+        <v>9</v>
+      </c>
+      <c r="I39" t="s">
+        <v>9</v>
+      </c>
+      <c r="L39" t="s">
+        <v>29</v>
+      </c>
+      <c r="M39">
+        <v>1.8580000000000001</v>
+      </c>
+      <c r="N39" t="s">
+        <v>9</v>
+      </c>
+      <c r="O39" t="s">
+        <v>9</v>
+      </c>
+      <c r="P39">
+        <v>2.7559999999999998</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>9</v>
+      </c>
+      <c r="R39" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
+        <v>15</v>
+      </c>
+      <c r="C40" t="s">
+        <v>24</v>
+      </c>
+      <c r="D40" t="s">
+        <v>50</v>
+      </c>
+      <c r="E40" t="s">
+        <v>9</v>
+      </c>
+      <c r="F40" t="s">
+        <v>51</v>
+      </c>
+      <c r="G40" t="s">
+        <v>52</v>
+      </c>
+      <c r="H40" t="s">
+        <v>9</v>
+      </c>
+      <c r="I40" t="s">
+        <v>9</v>
+      </c>
+      <c r="K40" t="s">
+        <v>365</v>
+      </c>
+      <c r="L40" t="s">
+        <v>24</v>
+      </c>
+      <c r="M40" t="s">
+        <v>366</v>
+      </c>
+      <c r="N40" t="s">
+        <v>395</v>
+      </c>
+      <c r="O40" t="s">
+        <v>177</v>
+      </c>
+      <c r="P40" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>9</v>
+      </c>
+      <c r="R40" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C41" t="s">
+        <v>29</v>
+      </c>
+      <c r="D41">
+        <v>0.63100000000000001</v>
+      </c>
+      <c r="E41" t="s">
+        <v>9</v>
+      </c>
+      <c r="F41">
+        <v>0.496</v>
+      </c>
+      <c r="G41">
+        <v>1.986</v>
+      </c>
+      <c r="H41" t="s">
+        <v>9</v>
+      </c>
+      <c r="I41" t="s">
+        <v>9</v>
+      </c>
+      <c r="L41" t="s">
+        <v>29</v>
+      </c>
+      <c r="M41">
+        <v>2.1669999999999998</v>
+      </c>
+      <c r="N41">
+        <v>91.95</v>
+      </c>
+      <c r="O41">
+        <v>11.717000000000001</v>
+      </c>
+      <c r="P41" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>9</v>
+      </c>
+      <c r="R41" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
+        <v>16</v>
+      </c>
+      <c r="C42" t="s">
+        <v>24</v>
+      </c>
+      <c r="D42" t="s">
+        <v>53</v>
+      </c>
+      <c r="E42" t="s">
+        <v>54</v>
+      </c>
+      <c r="F42" t="s">
+        <v>55</v>
+      </c>
+      <c r="G42" t="s">
+        <v>56</v>
+      </c>
+      <c r="H42" t="s">
+        <v>9</v>
+      </c>
+      <c r="I42" t="s">
+        <v>9</v>
+      </c>
+      <c r="K42" t="s">
+        <v>262</v>
+      </c>
+      <c r="L42" t="s">
+        <v>24</v>
+      </c>
+      <c r="M42" t="s">
+        <v>338</v>
+      </c>
+      <c r="N42" t="s">
+        <v>335</v>
+      </c>
+      <c r="O42" t="s">
+        <v>336</v>
+      </c>
+      <c r="P42" t="s">
+        <v>396</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>334</v>
+      </c>
+      <c r="R42" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="43" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C43" t="s">
+        <v>29</v>
+      </c>
+      <c r="D43">
+        <v>0.72099999999999997</v>
+      </c>
+      <c r="E43">
+        <v>19.347999999999999</v>
+      </c>
+      <c r="F43">
+        <v>3.3479999999999999</v>
+      </c>
+      <c r="G43">
+        <v>42.173000000000002</v>
+      </c>
+      <c r="H43" t="s">
+        <v>9</v>
+      </c>
+      <c r="I43" t="s">
+        <v>9</v>
+      </c>
+      <c r="L43" t="s">
+        <v>29</v>
+      </c>
+      <c r="M43">
+        <v>2.4769999999999999</v>
+      </c>
+      <c r="N43">
+        <v>11.455</v>
+      </c>
+      <c r="O43">
+        <v>8.1739999999999995</v>
+      </c>
+      <c r="P43">
+        <v>6.6929999999999996</v>
+      </c>
+      <c r="Q43">
+        <v>2.7589999999999999</v>
+      </c>
+      <c r="R43">
+        <v>84.066000000000003</v>
+      </c>
+    </row>
+    <row r="44" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B44" t="s">
+        <v>17</v>
+      </c>
+      <c r="C44" t="s">
+        <v>24</v>
+      </c>
+      <c r="D44" t="s">
+        <v>57</v>
+      </c>
+      <c r="E44" t="s">
+        <v>58</v>
+      </c>
+      <c r="F44" t="s">
+        <v>59</v>
+      </c>
+      <c r="G44" t="s">
+        <v>60</v>
+      </c>
+      <c r="H44" t="s">
+        <v>61</v>
+      </c>
+      <c r="I44" t="s">
+        <v>9</v>
+      </c>
+      <c r="K44" t="s">
+        <v>371</v>
+      </c>
+      <c r="L44" t="s">
+        <v>24</v>
+      </c>
+      <c r="M44" t="s">
+        <v>372</v>
+      </c>
+      <c r="N44" t="s">
+        <v>373</v>
+      </c>
+      <c r="O44" t="s">
+        <v>374</v>
+      </c>
+      <c r="P44" t="s">
+        <v>398</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>9</v>
+      </c>
+      <c r="R44" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C45" t="s">
+        <v>29</v>
+      </c>
+      <c r="D45">
+        <v>0.81200000000000006</v>
+      </c>
+      <c r="E45">
+        <v>1.276</v>
+      </c>
+      <c r="F45">
+        <v>1.984</v>
+      </c>
+      <c r="G45">
+        <v>7.593</v>
+      </c>
+      <c r="H45">
+        <v>13.565</v>
+      </c>
+      <c r="I45" t="s">
+        <v>9</v>
+      </c>
+      <c r="L45" t="s">
+        <v>29</v>
+      </c>
+      <c r="M45">
+        <v>2.786</v>
+      </c>
+      <c r="N45">
+        <v>59.442999999999998</v>
+      </c>
+      <c r="O45">
+        <v>14.169</v>
+      </c>
+      <c r="P45">
+        <v>5.9059999999999997</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>9</v>
+      </c>
+      <c r="R45" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B46" t="s">
+        <v>18</v>
+      </c>
+      <c r="C46" t="s">
+        <v>24</v>
+      </c>
+      <c r="D46" t="s">
+        <v>62</v>
+      </c>
+      <c r="E46" t="s">
+        <v>9</v>
+      </c>
+      <c r="F46" t="s">
+        <v>63</v>
+      </c>
+      <c r="G46" t="s">
+        <v>64</v>
+      </c>
+      <c r="H46" t="s">
+        <v>9</v>
+      </c>
+      <c r="I46" t="s">
+        <v>9</v>
+      </c>
+      <c r="K46" t="s">
+        <v>376</v>
+      </c>
+      <c r="L46" t="s">
+        <v>24</v>
+      </c>
+      <c r="M46" t="s">
+        <v>377</v>
+      </c>
+      <c r="N46" t="s">
+        <v>378</v>
+      </c>
+      <c r="O46" t="s">
+        <v>379</v>
+      </c>
+      <c r="P46" t="s">
+        <v>399</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>9</v>
+      </c>
+      <c r="R46" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C47" t="s">
+        <v>29</v>
+      </c>
+      <c r="D47">
+        <v>0.90200000000000002</v>
+      </c>
+      <c r="E47" t="s">
+        <v>9</v>
+      </c>
+      <c r="F47">
+        <v>55.115000000000002</v>
+      </c>
+      <c r="G47">
+        <v>10.164</v>
+      </c>
+      <c r="H47" t="s">
+        <v>9</v>
+      </c>
+      <c r="I47" t="s">
+        <v>9</v>
+      </c>
+      <c r="L47" t="s">
+        <v>29</v>
+      </c>
+      <c r="M47">
+        <v>3.0960000000000001</v>
+      </c>
+      <c r="N47">
+        <v>85.448999999999998</v>
+      </c>
+      <c r="O47">
+        <v>56.402999999999999</v>
+      </c>
+      <c r="P47">
+        <v>14.961</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>9</v>
+      </c>
+      <c r="R47" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B48" t="s">
+        <v>19</v>
+      </c>
+      <c r="C48" t="s">
+        <v>24</v>
+      </c>
+      <c r="D48" t="s">
+        <v>62</v>
+      </c>
+      <c r="E48" t="s">
+        <v>26</v>
+      </c>
+      <c r="F48" t="s">
+        <v>26</v>
+      </c>
+      <c r="G48" t="s">
+        <v>65</v>
+      </c>
+      <c r="H48" t="s">
+        <v>9</v>
+      </c>
+      <c r="I48" t="s">
+        <v>9</v>
+      </c>
+      <c r="K48" t="s">
+        <v>295</v>
+      </c>
+      <c r="L48" t="s">
+        <v>24</v>
+      </c>
+      <c r="M48" t="s">
+        <v>300</v>
+      </c>
+      <c r="N48" t="s">
+        <v>297</v>
+      </c>
+      <c r="O48" t="s">
+        <v>298</v>
+      </c>
+      <c r="P48" t="s">
+        <v>381</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>296</v>
+      </c>
+      <c r="R48" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="49" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C49" t="s">
+        <v>29</v>
+      </c>
+      <c r="D49">
+        <v>0.99199999999999999</v>
+      </c>
+      <c r="E49">
+        <v>68.037000000000006</v>
+      </c>
+      <c r="F49">
+        <v>79.230999999999995</v>
+      </c>
+      <c r="G49">
+        <v>8.4109999999999996</v>
+      </c>
+      <c r="H49" t="s">
+        <v>9</v>
+      </c>
+      <c r="I49" t="s">
+        <v>9</v>
+      </c>
+      <c r="L49" t="s">
+        <v>29</v>
+      </c>
+      <c r="M49">
+        <v>3.4060000000000001</v>
+      </c>
+      <c r="N49">
+        <v>87.926000000000002</v>
+      </c>
+      <c r="O49">
+        <v>41.417000000000002</v>
+      </c>
+      <c r="P49">
+        <v>7.8739999999999997</v>
+      </c>
+      <c r="Q49">
+        <v>0.69</v>
+      </c>
+      <c r="R49">
+        <v>14.835000000000001</v>
+      </c>
+    </row>
+    <row r="50" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B50" t="s">
+        <v>20</v>
+      </c>
+      <c r="C50" t="s">
+        <v>24</v>
+      </c>
+      <c r="D50" t="s">
+        <v>48</v>
+      </c>
+      <c r="E50" t="s">
+        <v>66</v>
+      </c>
+      <c r="F50" t="s">
+        <v>67</v>
+      </c>
+      <c r="G50" t="s">
+        <v>68</v>
+      </c>
+      <c r="H50" t="s">
+        <v>9</v>
+      </c>
+      <c r="I50" t="s">
+        <v>9</v>
+      </c>
+      <c r="K50" t="s">
+        <v>383</v>
+      </c>
+      <c r="L50" t="s">
+        <v>24</v>
+      </c>
+      <c r="M50" t="s">
+        <v>384</v>
+      </c>
+      <c r="N50" t="s">
+        <v>9</v>
+      </c>
+      <c r="O50" t="s">
+        <v>385</v>
+      </c>
+      <c r="P50" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>9</v>
+      </c>
+      <c r="R50" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C51" t="s">
+        <v>29</v>
+      </c>
+      <c r="D51">
+        <v>1.0820000000000001</v>
+      </c>
+      <c r="E51">
+        <v>2.5510000000000002</v>
+      </c>
+      <c r="F51">
+        <v>11.035</v>
+      </c>
+      <c r="G51">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="H51" t="s">
+        <v>9</v>
+      </c>
+      <c r="I51" t="s">
+        <v>9</v>
+      </c>
+      <c r="L51" t="s">
+        <v>29</v>
+      </c>
+      <c r="M51">
+        <v>3.7149999999999999</v>
+      </c>
+      <c r="N51" t="s">
+        <v>9</v>
+      </c>
+      <c r="O51">
+        <v>94.822999999999993</v>
+      </c>
+      <c r="P51" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>9</v>
+      </c>
+      <c r="R51" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B52" t="s">
+        <v>21</v>
+      </c>
+      <c r="C52" t="s">
+        <v>24</v>
+      </c>
+      <c r="D52" t="s">
+        <v>69</v>
+      </c>
+      <c r="E52" t="s">
+        <v>9</v>
+      </c>
+      <c r="F52" t="s">
+        <v>9</v>
+      </c>
+      <c r="G52" t="s">
+        <v>9</v>
+      </c>
+      <c r="H52" t="s">
+        <v>70</v>
+      </c>
+      <c r="I52" t="s">
+        <v>9</v>
+      </c>
+      <c r="K52" t="s">
+        <v>387</v>
+      </c>
+      <c r="L52" t="s">
+        <v>24</v>
+      </c>
+      <c r="M52" t="s">
+        <v>388</v>
+      </c>
+      <c r="N52" t="s">
+        <v>9</v>
+      </c>
+      <c r="O52" t="s">
+        <v>9</v>
+      </c>
+      <c r="P52" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q52" t="s">
+        <v>9</v>
+      </c>
+      <c r="R52" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="53" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C53" t="s">
+        <v>29</v>
+      </c>
+      <c r="D53">
+        <v>1.1719999999999999</v>
+      </c>
+      <c r="E53" t="s">
+        <v>9</v>
+      </c>
+      <c r="F53" t="s">
+        <v>9</v>
+      </c>
+      <c r="G53" t="s">
+        <v>9</v>
+      </c>
+      <c r="H53">
+        <v>20.504999999999999</v>
+      </c>
+      <c r="I53" t="s">
+        <v>9</v>
+      </c>
+      <c r="L53" t="s">
+        <v>29</v>
+      </c>
+      <c r="M53">
+        <v>4.0250000000000004</v>
+      </c>
+      <c r="N53" t="s">
+        <v>9</v>
+      </c>
+      <c r="O53" t="s">
+        <v>9</v>
+      </c>
+      <c r="P53" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q53" t="s">
+        <v>9</v>
+      </c>
+      <c r="R53" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B54" t="s">
+        <v>22</v>
+      </c>
+      <c r="C54" t="s">
+        <v>24</v>
+      </c>
+      <c r="D54" t="s">
+        <v>71</v>
+      </c>
+      <c r="E54" t="s">
+        <v>72</v>
+      </c>
+      <c r="F54" t="s">
+        <v>73</v>
+      </c>
+      <c r="G54" t="s">
+        <v>74</v>
+      </c>
+      <c r="H54" t="s">
+        <v>75</v>
+      </c>
+      <c r="I54" t="s">
+        <v>76</v>
+      </c>
+      <c r="K54" t="s">
+        <v>328</v>
+      </c>
+      <c r="L54" t="s">
+        <v>24</v>
+      </c>
+      <c r="M54" t="s">
+        <v>333</v>
+      </c>
+      <c r="N54" t="s">
+        <v>330</v>
+      </c>
+      <c r="O54" t="s">
+        <v>331</v>
+      </c>
+      <c r="P54" t="s">
+        <v>401</v>
+      </c>
+      <c r="Q54" t="s">
+        <v>329</v>
+      </c>
+      <c r="R54" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C55" t="s">
+        <v>29</v>
+      </c>
+      <c r="D55">
+        <v>1.262</v>
+      </c>
+      <c r="E55">
+        <v>82.849000000000004</v>
+      </c>
+      <c r="F55">
+        <v>19.963000000000001</v>
+      </c>
+      <c r="G55">
+        <v>7.4770000000000003</v>
+      </c>
+      <c r="H55">
+        <v>5.2050000000000001</v>
+      </c>
+      <c r="I55">
+        <v>2.3210000000000002</v>
+      </c>
+      <c r="L55" t="s">
+        <v>29</v>
+      </c>
+      <c r="M55">
+        <v>4.3339999999999996</v>
+      </c>
+      <c r="N55">
+        <v>20.433</v>
+      </c>
+      <c r="O55">
+        <v>8.4469999999999992</v>
+      </c>
+      <c r="P55">
+        <v>8.2680000000000007</v>
+      </c>
+      <c r="Q55">
+        <v>2.069</v>
+      </c>
+      <c r="R55" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="56" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B56" t="s">
+        <v>23</v>
+      </c>
+      <c r="C56" t="s">
+        <v>24</v>
+      </c>
+      <c r="D56" t="s">
+        <v>77</v>
+      </c>
+      <c r="E56" t="s">
+        <v>78</v>
+      </c>
+      <c r="F56" t="s">
+        <v>79</v>
+      </c>
+      <c r="G56" t="s">
+        <v>80</v>
+      </c>
+      <c r="H56" t="s">
+        <v>81</v>
+      </c>
+      <c r="I56" t="s">
+        <v>402</v>
+      </c>
+      <c r="K56" t="s">
+        <v>389</v>
+      </c>
+      <c r="L56" t="s">
+        <v>24</v>
+      </c>
+      <c r="M56" t="s">
+        <v>390</v>
+      </c>
+      <c r="N56" t="s">
+        <v>391</v>
+      </c>
+      <c r="O56" t="s">
+        <v>392</v>
+      </c>
+      <c r="P56" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q56" t="s">
+        <v>9</v>
+      </c>
+      <c r="R56" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="57" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C57" t="s">
+        <v>29</v>
+      </c>
+      <c r="D57">
+        <v>1.353</v>
+      </c>
+      <c r="E57">
+        <v>37.066000000000003</v>
+      </c>
+      <c r="F57">
+        <v>43.954999999999998</v>
+      </c>
+      <c r="G57">
+        <v>59.695999999999998</v>
+      </c>
+      <c r="H57">
+        <v>15.930999999999999</v>
+      </c>
+      <c r="I57">
+        <v>54.851999999999997</v>
+      </c>
+      <c r="L57" t="s">
+        <v>29</v>
+      </c>
+      <c r="M57">
+        <v>4.6440000000000001</v>
+      </c>
+      <c r="N57">
+        <v>9.907</v>
+      </c>
+      <c r="O57">
+        <v>10.082000000000001</v>
+      </c>
+      <c r="P57" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q57" t="s">
+        <v>9</v>
+      </c>
+      <c r="R57" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="60" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B60" s="1"/>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B83" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>